<commit_message>
Changes in Test Data sheet
</commit_message>
<xml_diff>
--- a/A360Native_AutoQA/TestData/TestDataSheet.xlsx
+++ b/A360Native_AutoQA/TestData/TestDataSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A360\A360Native_AutoQA\A360Native_AutoQA\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BE7E79-0C66-49F9-9095-5E69E525BE9E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE561B3-F8E3-4BF9-9B7D-7A9F378B5A23}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="840" yWindow="3030" windowWidth="15375" windowHeight="7875" tabRatio="683" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="683" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="809">
   <si>
     <t>Project Name</t>
   </si>
@@ -3029,6 +3029,9 @@
   </si>
   <si>
     <t>MALIBU POKE</t>
+  </si>
+  <si>
+    <t>PRIME BAR</t>
   </si>
 </sst>
 </file>
@@ -4405,6 +4408,28 @@
     <xf numFmtId="0" fontId="12" fillId="10" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="68" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="68" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="68" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="10" borderId="68" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="68" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="68" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4447,11 +4472,22 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4464,39 +4500,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="68" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="68" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="68" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="10" borderId="68" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="68" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="68" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4881,33 +4884,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A1" s="149" t="s">
+      <c r="A1" s="159" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="150"/>
-      <c r="C1" s="150"/>
-      <c r="D1" s="150"/>
-      <c r="E1" s="151"/>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="161"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="152"/>
-      <c r="B2" s="153"/>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="154"/>
+      <c r="A2" s="162"/>
+      <c r="B2" s="163"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="163"/>
+      <c r="E2" s="164"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="155"/>
-      <c r="B3" s="156"/>
-      <c r="C3" s="156"/>
-      <c r="D3" s="156"/>
-      <c r="E3" s="157"/>
+      <c r="A3" s="165"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="166"/>
+      <c r="D3" s="166"/>
+      <c r="E3" s="167"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="2"/>
@@ -19098,7 +19101,7 @@
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19110,16 +19113,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" s="127" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="188" t="s">
+      <c r="A1" s="150" t="s">
         <v>772</v>
       </c>
-      <c r="B1" s="189" t="s">
+      <c r="B1" s="151" t="s">
         <v>773</v>
       </c>
-      <c r="C1" s="190" t="s">
+      <c r="C1" s="152" t="s">
         <v>774</v>
       </c>
-      <c r="D1" s="190" t="s">
+      <c r="D1" s="152" t="s">
         <v>792</v>
       </c>
       <c r="E1" s="146" t="s">
@@ -19128,99 +19131,102 @@
       <c r="F1" s="147" t="s">
         <v>804</v>
       </c>
-      <c r="G1" s="190" t="s">
+      <c r="G1" s="152" t="s">
         <v>794</v>
       </c>
-      <c r="H1" s="190" t="s">
+      <c r="H1" s="152" t="s">
         <v>797</v>
       </c>
-      <c r="I1" s="190" t="s">
+      <c r="I1" s="152" t="s">
         <v>795</v>
       </c>
-      <c r="J1" s="190" t="s">
+      <c r="J1" s="152" t="s">
         <v>796</v>
       </c>
-      <c r="K1" s="190" t="s">
+      <c r="K1" s="152" t="s">
         <v>793</v>
       </c>
-      <c r="L1" s="191" t="s">
+      <c r="L1" s="153" t="s">
         <v>775</v>
       </c>
-      <c r="M1" s="192" t="s">
+      <c r="M1" s="154" t="s">
         <v>776</v>
       </c>
-      <c r="N1" s="191" t="s">
+      <c r="N1" s="153" t="s">
         <v>769</v>
       </c>
-      <c r="O1" s="193" t="s">
+      <c r="O1" s="155" t="s">
         <v>777</v>
       </c>
-      <c r="P1" s="193" t="s">
+      <c r="P1" s="155" t="s">
         <v>778</v>
       </c>
-      <c r="Q1" s="188" t="s">
+      <c r="Q1" s="150" t="s">
         <v>779</v>
       </c>
-      <c r="R1" s="188" t="s">
+      <c r="R1" s="150" t="s">
         <v>780</v>
       </c>
-      <c r="S1" s="188" t="s">
+      <c r="S1" s="150" t="s">
         <v>781</v>
       </c>
-      <c r="T1" s="188" t="s">
+      <c r="T1" s="150" t="s">
         <v>782</v>
       </c>
-      <c r="U1" s="188" t="s">
+      <c r="U1" s="150" t="s">
         <v>783</v>
       </c>
-      <c r="V1" s="188" t="s">
+      <c r="V1" s="150" t="s">
         <v>784</v>
       </c>
-      <c r="W1" s="188" t="s">
+      <c r="W1" s="150" t="s">
         <v>785</v>
       </c>
-      <c r="X1" s="188" t="s">
+      <c r="X1" s="150" t="s">
         <v>786</v>
       </c>
-      <c r="Y1" s="188" t="s">
+      <c r="Y1" s="150" t="s">
         <v>787</v>
       </c>
-      <c r="Z1" s="194"/>
-      <c r="AA1" s="194"/>
-      <c r="AB1" s="194"/>
-      <c r="AC1" s="194"/>
-      <c r="AD1" s="194"/>
-      <c r="AE1" s="194"/>
-      <c r="AF1" s="194"/>
-      <c r="AG1" s="194"/>
-      <c r="AH1" s="194"/>
-    </row>
-    <row r="2" spans="1:34" s="195" customFormat="1">
-      <c r="A2" s="195">
+      <c r="Z1" s="156"/>
+      <c r="AA1" s="156"/>
+      <c r="AB1" s="156"/>
+      <c r="AC1" s="156"/>
+      <c r="AD1" s="156"/>
+      <c r="AE1" s="156"/>
+      <c r="AF1" s="156"/>
+      <c r="AG1" s="156"/>
+      <c r="AH1" s="156"/>
+    </row>
+    <row r="2" spans="1:34" s="157" customFormat="1">
+      <c r="A2" s="157">
         <v>1</v>
       </c>
-      <c r="B2" s="195" t="s">
+      <c r="B2" s="157" t="s">
         <v>802</v>
       </c>
-      <c r="C2" s="195" t="s">
+      <c r="C2" s="157" t="s">
         <v>801</v>
       </c>
-      <c r="D2" s="196" t="s">
+      <c r="D2" s="158" t="s">
         <v>798</v>
       </c>
-      <c r="E2" s="187" t="s">
+      <c r="E2" s="149" t="s">
         <v>805</v>
       </c>
-      <c r="F2" s="187" t="s">
+      <c r="F2" s="149" t="s">
         <v>806</v>
       </c>
-      <c r="G2" s="187" t="s">
+      <c r="G2" s="149" t="s">
         <v>807</v>
       </c>
-      <c r="M2" s="195">
+      <c r="H2" s="157" t="s">
+        <v>808</v>
+      </c>
+      <c r="M2" s="157">
         <v>15000</v>
       </c>
-      <c r="N2" s="195" t="b">
+      <c r="N2" s="157" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20314,12 +20320,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="27.75" customHeight="1">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="170" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="162"/>
+      <c r="B1" s="172"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="164" t="s">
+      <c r="D1" s="174" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -20353,10 +20359,10 @@
       <c r="Z1" s="7"/>
     </row>
     <row r="2" spans="1:26" ht="22.5" customHeight="1">
-      <c r="A2" s="161"/>
-      <c r="B2" s="163"/>
+      <c r="A2" s="171"/>
+      <c r="B2" s="173"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="165"/>
+      <c r="D2" s="175"/>
       <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
@@ -20388,14 +20394,14 @@
       <c r="Z2" s="7"/>
     </row>
     <row r="3" spans="1:26" ht="26.25" customHeight="1">
-      <c r="A3" s="167" t="s">
+      <c r="A3" s="177" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="168" t="s">
+      <c r="B3" s="178" t="s">
         <v>113</v>
       </c>
       <c r="C3" s="16"/>
-      <c r="D3" s="165"/>
+      <c r="D3" s="175"/>
       <c r="E3" s="4" t="s">
         <v>19</v>
       </c>
@@ -20427,10 +20433,10 @@
       <c r="Z3" s="7"/>
     </row>
     <row r="4" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A4" s="159"/>
-      <c r="B4" s="163"/>
+      <c r="A4" s="169"/>
+      <c r="B4" s="173"/>
       <c r="C4" s="16"/>
-      <c r="D4" s="166"/>
+      <c r="D4" s="176"/>
       <c r="E4" s="4" t="s">
         <v>22</v>
       </c>
@@ -20552,7 +20558,7 @@
       <c r="B7" s="48" t="s">
         <v>121</v>
       </c>
-      <c r="C7" s="169" t="s">
+      <c r="C7" s="179" t="s">
         <v>122</v>
       </c>
       <c r="D7" s="72"/>
@@ -20592,7 +20598,7 @@
     <row r="8" spans="1:26" ht="31.5" customHeight="1">
       <c r="A8" s="48"/>
       <c r="B8" s="48"/>
-      <c r="C8" s="170"/>
+      <c r="C8" s="180"/>
       <c r="D8" s="72"/>
       <c r="E8" s="51"/>
       <c r="F8" s="31"/>
@@ -20626,7 +20632,7 @@
       <c r="B9" s="48" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="159"/>
+      <c r="C9" s="169"/>
       <c r="D9" s="48"/>
       <c r="E9" s="7"/>
       <c r="F9" s="52" t="s">
@@ -20798,7 +20804,7 @@
       <c r="B14" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="C14" s="158" t="s">
+      <c r="C14" s="168" t="s">
         <v>140</v>
       </c>
       <c r="D14" s="72"/>
@@ -20836,7 +20842,7 @@
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="48"/>
       <c r="B15" s="53"/>
-      <c r="C15" s="159"/>
+      <c r="C15" s="169"/>
       <c r="D15" s="57"/>
       <c r="E15" s="57"/>
       <c r="F15" s="52" t="s">
@@ -30506,9 +30512,9 @@
       <c r="A1" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="176"/>
-      <c r="C1" s="186"/>
-      <c r="D1" s="167" t="s">
+      <c r="B1" s="191"/>
+      <c r="C1" s="183"/>
+      <c r="D1" s="177" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -30545,9 +30551,9 @@
     </row>
     <row r="2" spans="1:26" ht="22.5" customHeight="1">
       <c r="A2" s="80"/>
-      <c r="B2" s="159"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
+      <c r="B2" s="169"/>
+      <c r="C2" s="180"/>
+      <c r="D2" s="180"/>
       <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
@@ -30581,14 +30587,14 @@
       <c r="Z2" s="7"/>
     </row>
     <row r="3" spans="1:26" ht="23.25" customHeight="1">
-      <c r="A3" s="167" t="s">
+      <c r="A3" s="177" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="177" t="s">
+      <c r="B3" s="192" t="s">
         <v>204</v>
       </c>
-      <c r="C3" s="170"/>
-      <c r="D3" s="170"/>
+      <c r="C3" s="180"/>
+      <c r="D3" s="180"/>
       <c r="E3" s="4" t="s">
         <v>19</v>
       </c>
@@ -30620,10 +30626,10 @@
       <c r="Z3" s="7"/>
     </row>
     <row r="4" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A4" s="159"/>
-      <c r="B4" s="159"/>
-      <c r="C4" s="159"/>
-      <c r="D4" s="159"/>
+      <c r="A4" s="169"/>
+      <c r="B4" s="169"/>
+      <c r="C4" s="169"/>
+      <c r="D4" s="169"/>
       <c r="E4" s="4" t="s">
         <v>22</v>
       </c>
@@ -30739,13 +30745,13 @@
       <c r="Z6" s="6"/>
     </row>
     <row r="7" spans="1:26" ht="31.5" customHeight="1">
-      <c r="A7" s="171" t="s">
+      <c r="A7" s="181" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="173" t="s">
+      <c r="B7" s="184" t="s">
         <v>222</v>
       </c>
-      <c r="C7" s="171" t="s">
+      <c r="C7" s="181" t="s">
         <v>227</v>
       </c>
       <c r="D7" s="46" t="s">
@@ -30769,7 +30775,7 @@
       </c>
       <c r="K7" s="86"/>
       <c r="L7" s="86"/>
-      <c r="M7" s="171" t="s">
+      <c r="M7" s="181" t="s">
         <v>243</v>
       </c>
       <c r="N7" s="57"/>
@@ -30787,11 +30793,11 @@
       <c r="Z7" s="7"/>
     </row>
     <row r="8" spans="1:26" ht="42.75" customHeight="1">
-      <c r="A8" s="170"/>
-      <c r="B8" s="174"/>
-      <c r="C8" s="170"/>
+      <c r="A8" s="180"/>
+      <c r="B8" s="186"/>
+      <c r="C8" s="180"/>
       <c r="D8" s="52"/>
-      <c r="E8" s="182" t="s">
+      <c r="E8" s="187" t="s">
         <v>247</v>
       </c>
       <c r="F8" s="53" t="s">
@@ -30809,7 +30815,7 @@
       </c>
       <c r="K8" s="56"/>
       <c r="L8" s="56"/>
-      <c r="M8" s="170"/>
+      <c r="M8" s="180"/>
       <c r="N8" s="57"/>
       <c r="O8" s="7"/>
       <c r="P8" s="7"/>
@@ -30825,11 +30831,11 @@
       <c r="Z8" s="7"/>
     </row>
     <row r="9" spans="1:26" ht="130.5" customHeight="1">
-      <c r="A9" s="170"/>
-      <c r="B9" s="174"/>
-      <c r="C9" s="170"/>
+      <c r="A9" s="180"/>
+      <c r="B9" s="186"/>
+      <c r="C9" s="180"/>
       <c r="D9" s="31"/>
-      <c r="E9" s="170"/>
+      <c r="E9" s="180"/>
       <c r="F9" s="53" t="s">
         <v>72</v>
       </c>
@@ -30845,7 +30851,7 @@
       </c>
       <c r="K9" s="56"/>
       <c r="L9" s="56"/>
-      <c r="M9" s="170"/>
+      <c r="M9" s="180"/>
       <c r="N9" s="57"/>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
@@ -30861,11 +30867,11 @@
       <c r="Z9" s="7"/>
     </row>
     <row r="10" spans="1:26" ht="31.5" customHeight="1">
-      <c r="A10" s="170"/>
-      <c r="B10" s="174"/>
-      <c r="C10" s="170"/>
+      <c r="A10" s="180"/>
+      <c r="B10" s="186"/>
+      <c r="C10" s="180"/>
       <c r="D10" s="87"/>
-      <c r="E10" s="170"/>
+      <c r="E10" s="180"/>
       <c r="F10" s="53" t="s">
         <v>73</v>
       </c>
@@ -30881,7 +30887,7 @@
       </c>
       <c r="K10" s="56"/>
       <c r="L10" s="56"/>
-      <c r="M10" s="159"/>
+      <c r="M10" s="169"/>
       <c r="N10" s="57"/>
       <c r="O10" s="7"/>
       <c r="P10" s="7"/>
@@ -30897,11 +30903,11 @@
       <c r="Z10" s="7"/>
     </row>
     <row r="11" spans="1:26" ht="33" customHeight="1">
-      <c r="A11" s="172"/>
-      <c r="B11" s="175"/>
-      <c r="C11" s="172"/>
+      <c r="A11" s="182"/>
+      <c r="B11" s="185"/>
+      <c r="C11" s="182"/>
       <c r="D11" s="88"/>
-      <c r="E11" s="172"/>
+      <c r="E11" s="182"/>
       <c r="F11" s="63" t="s">
         <v>74</v>
       </c>
@@ -30935,17 +30941,17 @@
       <c r="Z11" s="7"/>
     </row>
     <row r="12" spans="1:26" ht="215.25" customHeight="1">
-      <c r="A12" s="171" t="s">
+      <c r="A12" s="181" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="173" t="s">
+      <c r="B12" s="184" t="s">
         <v>279</v>
       </c>
-      <c r="C12" s="171" t="s">
+      <c r="C12" s="181" t="s">
         <v>282</v>
       </c>
       <c r="D12" s="92"/>
-      <c r="E12" s="171" t="s">
+      <c r="E12" s="181" t="s">
         <v>285</v>
       </c>
       <c r="F12" s="46" t="s">
@@ -30963,7 +30969,7 @@
       </c>
       <c r="K12" s="86"/>
       <c r="L12" s="86"/>
-      <c r="M12" s="171" t="s">
+      <c r="M12" s="181" t="s">
         <v>296</v>
       </c>
       <c r="N12" s="57"/>
@@ -30981,11 +30987,11 @@
       <c r="Z12" s="7"/>
     </row>
     <row r="13" spans="1:26" ht="33" customHeight="1">
-      <c r="A13" s="170"/>
-      <c r="B13" s="174"/>
-      <c r="C13" s="170"/>
+      <c r="A13" s="180"/>
+      <c r="B13" s="186"/>
+      <c r="C13" s="180"/>
       <c r="D13" s="72"/>
-      <c r="E13" s="170"/>
+      <c r="E13" s="180"/>
       <c r="F13" s="53" t="s">
         <v>76</v>
       </c>
@@ -31001,7 +31007,7 @@
       </c>
       <c r="K13" s="56"/>
       <c r="L13" s="56"/>
-      <c r="M13" s="170"/>
+      <c r="M13" s="180"/>
       <c r="N13" s="57"/>
       <c r="O13" s="7"/>
       <c r="P13" s="7"/>
@@ -31017,11 +31023,11 @@
       <c r="Z13" s="7"/>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="170"/>
-      <c r="B14" s="174"/>
-      <c r="C14" s="170"/>
+      <c r="A14" s="180"/>
+      <c r="B14" s="186"/>
+      <c r="C14" s="180"/>
       <c r="D14" s="57"/>
-      <c r="E14" s="170"/>
+      <c r="E14" s="180"/>
       <c r="F14" s="53" t="s">
         <v>77</v>
       </c>
@@ -31037,7 +31043,7 @@
       </c>
       <c r="K14" s="57"/>
       <c r="L14" s="56"/>
-      <c r="M14" s="170"/>
+      <c r="M14" s="180"/>
       <c r="N14" s="57"/>
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
@@ -31053,11 +31059,11 @@
       <c r="Z14" s="7"/>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" s="170"/>
-      <c r="B15" s="174"/>
-      <c r="C15" s="170"/>
+      <c r="A15" s="180"/>
+      <c r="B15" s="186"/>
+      <c r="C15" s="180"/>
       <c r="D15" s="57"/>
-      <c r="E15" s="170"/>
+      <c r="E15" s="180"/>
       <c r="F15" s="53" t="s">
         <v>78</v>
       </c>
@@ -31073,7 +31079,7 @@
       </c>
       <c r="K15" s="57"/>
       <c r="L15" s="56"/>
-      <c r="M15" s="170"/>
+      <c r="M15" s="180"/>
       <c r="N15" s="57"/>
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
@@ -31089,11 +31095,11 @@
       <c r="Z15" s="7"/>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" s="172"/>
-      <c r="B16" s="175"/>
-      <c r="C16" s="172"/>
+      <c r="A16" s="182"/>
+      <c r="B16" s="185"/>
+      <c r="C16" s="182"/>
       <c r="D16" s="94"/>
-      <c r="E16" s="172"/>
+      <c r="E16" s="182"/>
       <c r="F16" s="63" t="s">
         <v>79</v>
       </c>
@@ -31109,7 +31115,7 @@
       </c>
       <c r="K16" s="94"/>
       <c r="L16" s="89"/>
-      <c r="M16" s="172"/>
+      <c r="M16" s="182"/>
       <c r="N16" s="57"/>
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
@@ -31171,17 +31177,17 @@
       <c r="Z17" s="7"/>
     </row>
     <row r="18" spans="1:26" ht="28.5" customHeight="1">
-      <c r="A18" s="171" t="s">
+      <c r="A18" s="181" t="s">
         <v>101</v>
       </c>
-      <c r="B18" s="173" t="s">
+      <c r="B18" s="184" t="s">
         <v>349</v>
       </c>
-      <c r="C18" s="171" t="s">
+      <c r="C18" s="181" t="s">
         <v>354</v>
       </c>
       <c r="D18" s="85"/>
-      <c r="E18" s="183" t="s">
+      <c r="E18" s="188" t="s">
         <v>285</v>
       </c>
       <c r="F18" s="46" t="s">
@@ -31199,7 +31205,7 @@
       </c>
       <c r="K18" s="85"/>
       <c r="L18" s="86"/>
-      <c r="M18" s="171" t="s">
+      <c r="M18" s="181" t="s">
         <v>296</v>
       </c>
       <c r="N18" s="57"/>
@@ -31217,11 +31223,11 @@
       <c r="Z18" s="7"/>
     </row>
     <row r="19" spans="1:26" ht="22.5" customHeight="1">
-      <c r="A19" s="170"/>
-      <c r="B19" s="174"/>
-      <c r="C19" s="170"/>
+      <c r="A19" s="180"/>
+      <c r="B19" s="186"/>
+      <c r="C19" s="180"/>
       <c r="D19" s="57"/>
-      <c r="E19" s="184"/>
+      <c r="E19" s="189"/>
       <c r="F19" s="53" t="s">
         <v>82</v>
       </c>
@@ -31237,7 +31243,7 @@
       </c>
       <c r="K19" s="57"/>
       <c r="L19" s="56"/>
-      <c r="M19" s="170"/>
+      <c r="M19" s="180"/>
       <c r="N19" s="57"/>
       <c r="O19" s="7"/>
       <c r="P19" s="7"/>
@@ -31253,11 +31259,11 @@
       <c r="Z19" s="7"/>
     </row>
     <row r="20" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A20" s="170"/>
-      <c r="B20" s="174"/>
-      <c r="C20" s="170"/>
+      <c r="A20" s="180"/>
+      <c r="B20" s="186"/>
+      <c r="C20" s="180"/>
       <c r="D20" s="57"/>
-      <c r="E20" s="184"/>
+      <c r="E20" s="189"/>
       <c r="F20" s="53" t="s">
         <v>84</v>
       </c>
@@ -31273,7 +31279,7 @@
       </c>
       <c r="K20" s="57"/>
       <c r="L20" s="56"/>
-      <c r="M20" s="170"/>
+      <c r="M20" s="180"/>
       <c r="N20" s="57"/>
       <c r="O20" s="7"/>
       <c r="P20" s="7"/>
@@ -31289,11 +31295,11 @@
       <c r="Z20" s="7"/>
     </row>
     <row r="21" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A21" s="172"/>
-      <c r="B21" s="175"/>
-      <c r="C21" s="172"/>
+      <c r="A21" s="182"/>
+      <c r="B21" s="185"/>
+      <c r="C21" s="182"/>
       <c r="D21" s="94"/>
-      <c r="E21" s="185"/>
+      <c r="E21" s="190"/>
       <c r="F21" s="63" t="s">
         <v>85</v>
       </c>
@@ -31309,7 +31315,7 @@
       </c>
       <c r="K21" s="94"/>
       <c r="L21" s="89"/>
-      <c r="M21" s="172"/>
+      <c r="M21" s="182"/>
       <c r="N21" s="57"/>
       <c r="O21" s="7"/>
       <c r="P21" s="7"/>
@@ -31325,13 +31331,13 @@
       <c r="Z21" s="7"/>
     </row>
     <row r="22" spans="1:26" ht="29.25" customHeight="1">
-      <c r="A22" s="171" t="s">
+      <c r="A22" s="181" t="s">
         <v>104</v>
       </c>
-      <c r="B22" s="173" t="s">
+      <c r="B22" s="184" t="s">
         <v>386</v>
       </c>
-      <c r="C22" s="171" t="s">
+      <c r="C22" s="181" t="s">
         <v>388</v>
       </c>
       <c r="D22" s="85"/>
@@ -31353,7 +31359,7 @@
       </c>
       <c r="K22" s="85"/>
       <c r="L22" s="86"/>
-      <c r="M22" s="171" t="s">
+      <c r="M22" s="181" t="s">
         <v>393</v>
       </c>
       <c r="N22" s="57"/>
@@ -31371,11 +31377,11 @@
       <c r="Z22" s="7"/>
     </row>
     <row r="23" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A23" s="170"/>
-      <c r="B23" s="174"/>
-      <c r="C23" s="170"/>
+      <c r="A23" s="180"/>
+      <c r="B23" s="186"/>
+      <c r="C23" s="180"/>
       <c r="D23" s="57"/>
-      <c r="E23" s="182" t="s">
+      <c r="E23" s="187" t="s">
         <v>398</v>
       </c>
       <c r="F23" s="53" t="s">
@@ -31393,7 +31399,7 @@
       </c>
       <c r="K23" s="57"/>
       <c r="L23" s="56"/>
-      <c r="M23" s="170"/>
+      <c r="M23" s="180"/>
       <c r="N23" s="57"/>
       <c r="O23" s="7"/>
       <c r="P23" s="7"/>
@@ -31409,11 +31415,11 @@
       <c r="Z23" s="7"/>
     </row>
     <row r="24" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A24" s="170"/>
-      <c r="B24" s="174"/>
-      <c r="C24" s="170"/>
+      <c r="A24" s="180"/>
+      <c r="B24" s="186"/>
+      <c r="C24" s="180"/>
       <c r="D24" s="57"/>
-      <c r="E24" s="170"/>
+      <c r="E24" s="180"/>
       <c r="F24" s="53" t="s">
         <v>91</v>
       </c>
@@ -31429,7 +31435,7 @@
       </c>
       <c r="K24" s="57"/>
       <c r="L24" s="56"/>
-      <c r="M24" s="170"/>
+      <c r="M24" s="180"/>
       <c r="N24" s="57"/>
       <c r="O24" s="7"/>
       <c r="P24" s="7"/>
@@ -31445,11 +31451,11 @@
       <c r="Z24" s="7"/>
     </row>
     <row r="25" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A25" s="170"/>
-      <c r="B25" s="174"/>
-      <c r="C25" s="170"/>
+      <c r="A25" s="180"/>
+      <c r="B25" s="186"/>
+      <c r="C25" s="180"/>
       <c r="D25" s="57"/>
-      <c r="E25" s="170"/>
+      <c r="E25" s="180"/>
       <c r="F25" s="53" t="s">
         <v>92</v>
       </c>
@@ -31465,7 +31471,7 @@
       </c>
       <c r="K25" s="57"/>
       <c r="L25" s="56"/>
-      <c r="M25" s="170"/>
+      <c r="M25" s="180"/>
       <c r="N25" s="57"/>
       <c r="O25" s="7"/>
       <c r="P25" s="7"/>
@@ -31481,11 +31487,11 @@
       <c r="Z25" s="7"/>
     </row>
     <row r="26" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A26" s="170"/>
-      <c r="B26" s="174"/>
-      <c r="C26" s="170"/>
+      <c r="A26" s="180"/>
+      <c r="B26" s="186"/>
+      <c r="C26" s="180"/>
       <c r="D26" s="57"/>
-      <c r="E26" s="170"/>
+      <c r="E26" s="180"/>
       <c r="F26" s="53" t="s">
         <v>93</v>
       </c>
@@ -31501,7 +31507,7 @@
       </c>
       <c r="K26" s="57"/>
       <c r="L26" s="56"/>
-      <c r="M26" s="170"/>
+      <c r="M26" s="180"/>
       <c r="N26" s="57"/>
       <c r="O26" s="7"/>
       <c r="P26" s="7"/>
@@ -31517,11 +31523,11 @@
       <c r="Z26" s="7"/>
     </row>
     <row r="27" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A27" s="170"/>
-      <c r="B27" s="174"/>
-      <c r="C27" s="170"/>
+      <c r="A27" s="180"/>
+      <c r="B27" s="186"/>
+      <c r="C27" s="180"/>
       <c r="D27" s="57"/>
-      <c r="E27" s="170"/>
+      <c r="E27" s="180"/>
       <c r="F27" s="53" t="s">
         <v>94</v>
       </c>
@@ -31537,7 +31543,7 @@
       </c>
       <c r="K27" s="57"/>
       <c r="L27" s="56"/>
-      <c r="M27" s="170"/>
+      <c r="M27" s="180"/>
       <c r="N27" s="57"/>
       <c r="O27" s="7"/>
       <c r="P27" s="7"/>
@@ -31553,11 +31559,11 @@
       <c r="Z27" s="7"/>
     </row>
     <row r="28" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A28" s="170"/>
-      <c r="B28" s="174"/>
-      <c r="C28" s="170"/>
+      <c r="A28" s="180"/>
+      <c r="B28" s="186"/>
+      <c r="C28" s="180"/>
       <c r="D28" s="57"/>
-      <c r="E28" s="170"/>
+      <c r="E28" s="180"/>
       <c r="F28" s="53" t="s">
         <v>95</v>
       </c>
@@ -31573,7 +31579,7 @@
       </c>
       <c r="K28" s="57"/>
       <c r="L28" s="56"/>
-      <c r="M28" s="170"/>
+      <c r="M28" s="180"/>
       <c r="N28" s="57"/>
       <c r="O28" s="7"/>
       <c r="P28" s="7"/>
@@ -31589,11 +31595,11 @@
       <c r="Z28" s="7"/>
     </row>
     <row r="29" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A29" s="170"/>
-      <c r="B29" s="174"/>
-      <c r="C29" s="170"/>
+      <c r="A29" s="180"/>
+      <c r="B29" s="186"/>
+      <c r="C29" s="180"/>
       <c r="D29" s="57"/>
-      <c r="E29" s="170"/>
+      <c r="E29" s="180"/>
       <c r="F29" s="53" t="s">
         <v>96</v>
       </c>
@@ -31609,7 +31615,7 @@
       </c>
       <c r="K29" s="57"/>
       <c r="L29" s="56"/>
-      <c r="M29" s="170"/>
+      <c r="M29" s="180"/>
       <c r="N29" s="57"/>
       <c r="O29" s="7"/>
       <c r="P29" s="7"/>
@@ -31625,11 +31631,11 @@
       <c r="Z29" s="7"/>
     </row>
     <row r="30" spans="1:26" ht="21" customHeight="1">
-      <c r="A30" s="170"/>
-      <c r="B30" s="174"/>
-      <c r="C30" s="170"/>
+      <c r="A30" s="180"/>
+      <c r="B30" s="186"/>
+      <c r="C30" s="180"/>
       <c r="D30" s="57"/>
-      <c r="E30" s="170"/>
+      <c r="E30" s="180"/>
       <c r="F30" s="53" t="s">
         <v>99</v>
       </c>
@@ -31645,7 +31651,7 @@
       </c>
       <c r="K30" s="57"/>
       <c r="L30" s="56"/>
-      <c r="M30" s="170"/>
+      <c r="M30" s="180"/>
       <c r="N30" s="57"/>
       <c r="O30" s="7"/>
       <c r="P30" s="7"/>
@@ -31661,11 +31667,11 @@
       <c r="Z30" s="7"/>
     </row>
     <row r="31" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A31" s="170"/>
-      <c r="B31" s="174"/>
-      <c r="C31" s="170"/>
+      <c r="A31" s="180"/>
+      <c r="B31" s="186"/>
+      <c r="C31" s="180"/>
       <c r="D31" s="57"/>
-      <c r="E31" s="170"/>
+      <c r="E31" s="180"/>
       <c r="F31" s="53" t="s">
         <v>100</v>
       </c>
@@ -31681,7 +31687,7 @@
       </c>
       <c r="K31" s="57"/>
       <c r="L31" s="56"/>
-      <c r="M31" s="159"/>
+      <c r="M31" s="169"/>
       <c r="N31" s="57"/>
       <c r="O31" s="7"/>
       <c r="P31" s="7"/>
@@ -31697,11 +31703,11 @@
       <c r="Z31" s="7"/>
     </row>
     <row r="32" spans="1:26" ht="33.75" customHeight="1">
-      <c r="A32" s="170"/>
-      <c r="B32" s="174"/>
-      <c r="C32" s="170"/>
+      <c r="A32" s="180"/>
+      <c r="B32" s="186"/>
+      <c r="C32" s="180"/>
       <c r="D32" s="67"/>
-      <c r="E32" s="170"/>
+      <c r="E32" s="180"/>
       <c r="F32" s="93" t="s">
         <v>102</v>
       </c>
@@ -31735,17 +31741,17 @@
       <c r="Z32" s="7"/>
     </row>
     <row r="33" spans="1:26" ht="32.25" customHeight="1">
-      <c r="A33" s="171" t="s">
+      <c r="A33" s="181" t="s">
         <v>111</v>
       </c>
-      <c r="B33" s="173" t="s">
+      <c r="B33" s="184" t="s">
         <v>450</v>
       </c>
-      <c r="C33" s="171" t="s">
+      <c r="C33" s="181" t="s">
         <v>452</v>
       </c>
       <c r="D33" s="85"/>
-      <c r="E33" s="171" t="s">
+      <c r="E33" s="181" t="s">
         <v>398</v>
       </c>
       <c r="F33" s="46" t="s">
@@ -31763,7 +31769,7 @@
       </c>
       <c r="K33" s="85"/>
       <c r="L33" s="86"/>
-      <c r="M33" s="171" t="s">
+      <c r="M33" s="181" t="s">
         <v>393</v>
       </c>
       <c r="N33" s="102"/>
@@ -31781,11 +31787,11 @@
       <c r="Z33" s="7"/>
     </row>
     <row r="34" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A34" s="170"/>
-      <c r="B34" s="174"/>
-      <c r="C34" s="170"/>
+      <c r="A34" s="180"/>
+      <c r="B34" s="186"/>
+      <c r="C34" s="180"/>
       <c r="D34" s="57"/>
-      <c r="E34" s="170"/>
+      <c r="E34" s="180"/>
       <c r="F34" s="53" t="s">
         <v>105</v>
       </c>
@@ -31801,7 +31807,7 @@
       </c>
       <c r="K34" s="57"/>
       <c r="L34" s="56"/>
-      <c r="M34" s="170"/>
+      <c r="M34" s="180"/>
       <c r="N34" s="103"/>
       <c r="O34" s="7"/>
       <c r="P34" s="7"/>
@@ -31817,11 +31823,11 @@
       <c r="Z34" s="7"/>
     </row>
     <row r="35" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A35" s="170"/>
-      <c r="B35" s="174"/>
-      <c r="C35" s="170"/>
+      <c r="A35" s="180"/>
+      <c r="B35" s="186"/>
+      <c r="C35" s="180"/>
       <c r="D35" s="57"/>
-      <c r="E35" s="170"/>
+      <c r="E35" s="180"/>
       <c r="F35" s="53" t="s">
         <v>106</v>
       </c>
@@ -31837,7 +31843,7 @@
       </c>
       <c r="K35" s="57"/>
       <c r="L35" s="56"/>
-      <c r="M35" s="170"/>
+      <c r="M35" s="180"/>
       <c r="N35" s="103"/>
       <c r="O35" s="7"/>
       <c r="P35" s="7"/>
@@ -31853,11 +31859,11 @@
       <c r="Z35" s="7"/>
     </row>
     <row r="36" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A36" s="170"/>
-      <c r="B36" s="174"/>
-      <c r="C36" s="170"/>
+      <c r="A36" s="180"/>
+      <c r="B36" s="186"/>
+      <c r="C36" s="180"/>
       <c r="D36" s="67"/>
-      <c r="E36" s="170"/>
+      <c r="E36" s="180"/>
       <c r="F36" s="70" t="s">
         <v>107</v>
       </c>
@@ -31873,7 +31879,7 @@
       </c>
       <c r="K36" s="67"/>
       <c r="L36" s="75"/>
-      <c r="M36" s="170"/>
+      <c r="M36" s="180"/>
       <c r="N36" s="104"/>
       <c r="O36" s="7"/>
       <c r="P36" s="7"/>
@@ -31889,17 +31895,17 @@
       <c r="Z36" s="7"/>
     </row>
     <row r="37" spans="1:26" ht="30" customHeight="1">
-      <c r="A37" s="171" t="s">
+      <c r="A37" s="181" t="s">
         <v>130</v>
       </c>
-      <c r="B37" s="178" t="s">
+      <c r="B37" s="193" t="s">
         <v>470</v>
       </c>
-      <c r="C37" s="171" t="s">
+      <c r="C37" s="181" t="s">
         <v>472</v>
       </c>
       <c r="D37" s="85"/>
-      <c r="E37" s="171" t="s">
+      <c r="E37" s="181" t="s">
         <v>473</v>
       </c>
       <c r="F37" s="46" t="s">
@@ -31917,7 +31923,7 @@
       </c>
       <c r="K37" s="85"/>
       <c r="L37" s="86"/>
-      <c r="M37" s="171" t="s">
+      <c r="M37" s="181" t="s">
         <v>477</v>
       </c>
       <c r="N37" s="102"/>
@@ -31935,11 +31941,11 @@
       <c r="Z37" s="7"/>
     </row>
     <row r="38" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A38" s="170"/>
-      <c r="B38" s="179"/>
-      <c r="C38" s="170"/>
+      <c r="A38" s="180"/>
+      <c r="B38" s="194"/>
+      <c r="C38" s="180"/>
       <c r="D38" s="57"/>
-      <c r="E38" s="170"/>
+      <c r="E38" s="180"/>
       <c r="F38" s="53" t="s">
         <v>109</v>
       </c>
@@ -31955,7 +31961,7 @@
       </c>
       <c r="K38" s="57"/>
       <c r="L38" s="56"/>
-      <c r="M38" s="170"/>
+      <c r="M38" s="180"/>
       <c r="N38" s="103"/>
       <c r="O38" s="7"/>
       <c r="P38" s="7"/>
@@ -31971,11 +31977,11 @@
       <c r="Z38" s="7"/>
     </row>
     <row r="39" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A39" s="170"/>
-      <c r="B39" s="179"/>
-      <c r="C39" s="170"/>
+      <c r="A39" s="180"/>
+      <c r="B39" s="194"/>
+      <c r="C39" s="180"/>
       <c r="D39" s="57"/>
-      <c r="E39" s="170"/>
+      <c r="E39" s="180"/>
       <c r="F39" s="53" t="s">
         <v>110</v>
       </c>
@@ -31991,7 +31997,7 @@
       </c>
       <c r="K39" s="57"/>
       <c r="L39" s="56"/>
-      <c r="M39" s="170"/>
+      <c r="M39" s="180"/>
       <c r="N39" s="103"/>
       <c r="O39" s="7"/>
       <c r="P39" s="7"/>
@@ -32007,11 +32013,11 @@
       <c r="Z39" s="7"/>
     </row>
     <row r="40" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A40" s="170"/>
-      <c r="B40" s="179"/>
-      <c r="C40" s="170"/>
+      <c r="A40" s="180"/>
+      <c r="B40" s="194"/>
+      <c r="C40" s="180"/>
       <c r="D40" s="57"/>
-      <c r="E40" s="170"/>
+      <c r="E40" s="180"/>
       <c r="F40" s="53" t="s">
         <v>112</v>
       </c>
@@ -32027,7 +32033,7 @@
       </c>
       <c r="K40" s="57"/>
       <c r="L40" s="56"/>
-      <c r="M40" s="170"/>
+      <c r="M40" s="180"/>
       <c r="N40" s="103"/>
       <c r="O40" s="7"/>
       <c r="P40" s="7"/>
@@ -32043,11 +32049,11 @@
       <c r="Z40" s="7"/>
     </row>
     <row r="41" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A41" s="170"/>
-      <c r="B41" s="179"/>
-      <c r="C41" s="170"/>
+      <c r="A41" s="180"/>
+      <c r="B41" s="194"/>
+      <c r="C41" s="180"/>
       <c r="D41" s="57"/>
-      <c r="E41" s="170"/>
+      <c r="E41" s="180"/>
       <c r="F41" s="53" t="s">
         <v>114</v>
       </c>
@@ -32063,7 +32069,7 @@
       </c>
       <c r="K41" s="57"/>
       <c r="L41" s="56"/>
-      <c r="M41" s="170"/>
+      <c r="M41" s="180"/>
       <c r="N41" s="103"/>
       <c r="O41" s="7"/>
       <c r="P41" s="7"/>
@@ -32079,11 +32085,11 @@
       <c r="Z41" s="7"/>
     </row>
     <row r="42" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A42" s="170"/>
-      <c r="B42" s="179"/>
-      <c r="C42" s="170"/>
+      <c r="A42" s="180"/>
+      <c r="B42" s="194"/>
+      <c r="C42" s="180"/>
       <c r="D42" s="57"/>
-      <c r="E42" s="170"/>
+      <c r="E42" s="180"/>
       <c r="F42" s="53" t="s">
         <v>115</v>
       </c>
@@ -32099,7 +32105,7 @@
       </c>
       <c r="K42" s="57"/>
       <c r="L42" s="56"/>
-      <c r="M42" s="170"/>
+      <c r="M42" s="180"/>
       <c r="N42" s="103"/>
       <c r="O42" s="7"/>
       <c r="P42" s="7"/>
@@ -32115,11 +32121,11 @@
       <c r="Z42" s="7"/>
     </row>
     <row r="43" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A43" s="170"/>
-      <c r="B43" s="179"/>
-      <c r="C43" s="170"/>
+      <c r="A43" s="180"/>
+      <c r="B43" s="194"/>
+      <c r="C43" s="180"/>
       <c r="D43" s="57"/>
-      <c r="E43" s="170"/>
+      <c r="E43" s="180"/>
       <c r="F43" s="53" t="s">
         <v>116</v>
       </c>
@@ -32135,7 +32141,7 @@
       </c>
       <c r="K43" s="57"/>
       <c r="L43" s="56"/>
-      <c r="M43" s="170"/>
+      <c r="M43" s="180"/>
       <c r="N43" s="103"/>
       <c r="O43" s="7"/>
       <c r="P43" s="7"/>
@@ -32151,11 +32157,11 @@
       <c r="Z43" s="7"/>
     </row>
     <row r="44" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A44" s="170"/>
-      <c r="B44" s="179"/>
-      <c r="C44" s="170"/>
+      <c r="A44" s="180"/>
+      <c r="B44" s="194"/>
+      <c r="C44" s="180"/>
       <c r="D44" s="57"/>
-      <c r="E44" s="170"/>
+      <c r="E44" s="180"/>
       <c r="F44" s="53" t="s">
         <v>117</v>
       </c>
@@ -32171,7 +32177,7 @@
       </c>
       <c r="K44" s="57"/>
       <c r="L44" s="56"/>
-      <c r="M44" s="170"/>
+      <c r="M44" s="180"/>
       <c r="N44" s="103"/>
       <c r="O44" s="7"/>
       <c r="P44" s="7"/>
@@ -32187,11 +32193,11 @@
       <c r="Z44" s="7"/>
     </row>
     <row r="45" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A45" s="170"/>
-      <c r="B45" s="179"/>
-      <c r="C45" s="170"/>
+      <c r="A45" s="180"/>
+      <c r="B45" s="194"/>
+      <c r="C45" s="180"/>
       <c r="D45" s="57"/>
-      <c r="E45" s="170"/>
+      <c r="E45" s="180"/>
       <c r="F45" s="53" t="s">
         <v>118</v>
       </c>
@@ -32207,7 +32213,7 @@
       </c>
       <c r="K45" s="57"/>
       <c r="L45" s="56"/>
-      <c r="M45" s="170"/>
+      <c r="M45" s="180"/>
       <c r="N45" s="103"/>
       <c r="O45" s="7"/>
       <c r="P45" s="7"/>
@@ -32223,11 +32229,11 @@
       <c r="Z45" s="7"/>
     </row>
     <row r="46" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A46" s="170"/>
-      <c r="B46" s="179"/>
-      <c r="C46" s="170"/>
+      <c r="A46" s="180"/>
+      <c r="B46" s="194"/>
+      <c r="C46" s="180"/>
       <c r="D46" s="57"/>
-      <c r="E46" s="170"/>
+      <c r="E46" s="180"/>
       <c r="F46" s="105" t="s">
         <v>119</v>
       </c>
@@ -32243,7 +32249,7 @@
       </c>
       <c r="K46" s="57"/>
       <c r="L46" s="56"/>
-      <c r="M46" s="159"/>
+      <c r="M46" s="169"/>
       <c r="N46" s="103"/>
       <c r="O46" s="7"/>
       <c r="P46" s="7"/>
@@ -32259,11 +32265,11 @@
       <c r="Z46" s="7"/>
     </row>
     <row r="47" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A47" s="172"/>
-      <c r="B47" s="180"/>
-      <c r="C47" s="172"/>
+      <c r="A47" s="182"/>
+      <c r="B47" s="195"/>
+      <c r="C47" s="182"/>
       <c r="D47" s="94"/>
-      <c r="E47" s="172"/>
+      <c r="E47" s="182"/>
       <c r="F47" s="63" t="s">
         <v>120</v>
       </c>
@@ -32297,17 +32303,17 @@
       <c r="Z47" s="7"/>
     </row>
     <row r="48" spans="1:26" ht="45" customHeight="1">
-      <c r="A48" s="171" t="s">
+      <c r="A48" s="181" t="s">
         <v>254</v>
       </c>
-      <c r="B48" s="173" t="s">
+      <c r="B48" s="184" t="s">
         <v>500</v>
       </c>
-      <c r="C48" s="171" t="s">
+      <c r="C48" s="181" t="s">
         <v>501</v>
       </c>
       <c r="D48" s="85"/>
-      <c r="E48" s="171" t="s">
+      <c r="E48" s="181" t="s">
         <v>502</v>
       </c>
       <c r="F48" s="46" t="s">
@@ -32343,11 +32349,11 @@
       <c r="Z48" s="7"/>
     </row>
     <row r="49" spans="1:26" ht="30" customHeight="1">
-      <c r="A49" s="170"/>
-      <c r="B49" s="174"/>
-      <c r="C49" s="170"/>
+      <c r="A49" s="180"/>
+      <c r="B49" s="186"/>
+      <c r="C49" s="180"/>
       <c r="D49" s="57"/>
-      <c r="E49" s="170"/>
+      <c r="E49" s="180"/>
       <c r="F49" s="105" t="s">
         <v>135</v>
       </c>
@@ -32363,7 +32369,7 @@
       </c>
       <c r="K49" s="57"/>
       <c r="L49" s="56"/>
-      <c r="M49" s="171" t="s">
+      <c r="M49" s="181" t="s">
         <v>502</v>
       </c>
       <c r="N49" s="103"/>
@@ -32381,11 +32387,11 @@
       <c r="Z49" s="7"/>
     </row>
     <row r="50" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A50" s="170"/>
-      <c r="B50" s="174"/>
-      <c r="C50" s="170"/>
+      <c r="A50" s="180"/>
+      <c r="B50" s="186"/>
+      <c r="C50" s="180"/>
       <c r="D50" s="57"/>
-      <c r="E50" s="170"/>
+      <c r="E50" s="180"/>
       <c r="F50" s="105" t="s">
         <v>138</v>
       </c>
@@ -32401,7 +32407,7 @@
       </c>
       <c r="K50" s="57"/>
       <c r="L50" s="56"/>
-      <c r="M50" s="170"/>
+      <c r="M50" s="180"/>
       <c r="N50" s="103"/>
       <c r="O50" s="7"/>
       <c r="P50" s="7"/>
@@ -32417,11 +32423,11 @@
       <c r="Z50" s="7"/>
     </row>
     <row r="51" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A51" s="170"/>
-      <c r="B51" s="174"/>
-      <c r="C51" s="170"/>
+      <c r="A51" s="180"/>
+      <c r="B51" s="186"/>
+      <c r="C51" s="180"/>
       <c r="D51" s="57"/>
-      <c r="E51" s="170"/>
+      <c r="E51" s="180"/>
       <c r="F51" s="105" t="s">
         <v>144</v>
       </c>
@@ -32437,7 +32443,7 @@
       </c>
       <c r="K51" s="57"/>
       <c r="L51" s="56"/>
-      <c r="M51" s="170"/>
+      <c r="M51" s="180"/>
       <c r="N51" s="103"/>
       <c r="O51" s="7"/>
       <c r="P51" s="7"/>
@@ -32453,11 +32459,11 @@
       <c r="Z51" s="7"/>
     </row>
     <row r="52" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A52" s="170"/>
-      <c r="B52" s="174"/>
-      <c r="C52" s="170"/>
+      <c r="A52" s="180"/>
+      <c r="B52" s="186"/>
+      <c r="C52" s="180"/>
       <c r="D52" s="57"/>
-      <c r="E52" s="170"/>
+      <c r="E52" s="180"/>
       <c r="F52" s="105" t="s">
         <v>147</v>
       </c>
@@ -32473,7 +32479,7 @@
       </c>
       <c r="K52" s="57"/>
       <c r="L52" s="56"/>
-      <c r="M52" s="170"/>
+      <c r="M52" s="180"/>
       <c r="N52" s="103"/>
       <c r="O52" s="7"/>
       <c r="P52" s="7"/>
@@ -32489,11 +32495,11 @@
       <c r="Z52" s="7"/>
     </row>
     <row r="53" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A53" s="170"/>
-      <c r="B53" s="174"/>
-      <c r="C53" s="170"/>
+      <c r="A53" s="180"/>
+      <c r="B53" s="186"/>
+      <c r="C53" s="180"/>
       <c r="D53" s="57"/>
-      <c r="E53" s="170"/>
+      <c r="E53" s="180"/>
       <c r="F53" s="105" t="s">
         <v>150</v>
       </c>
@@ -32509,7 +32515,7 @@
       </c>
       <c r="K53" s="57"/>
       <c r="L53" s="56"/>
-      <c r="M53" s="170"/>
+      <c r="M53" s="180"/>
       <c r="N53" s="103"/>
       <c r="O53" s="7"/>
       <c r="P53" s="7"/>
@@ -32525,11 +32531,11 @@
       <c r="Z53" s="7"/>
     </row>
     <row r="54" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A54" s="170"/>
-      <c r="B54" s="174"/>
-      <c r="C54" s="170"/>
+      <c r="A54" s="180"/>
+      <c r="B54" s="186"/>
+      <c r="C54" s="180"/>
       <c r="D54" s="57"/>
-      <c r="E54" s="170"/>
+      <c r="E54" s="180"/>
       <c r="F54" s="105" t="s">
         <v>151</v>
       </c>
@@ -32545,7 +32551,7 @@
       </c>
       <c r="K54" s="57"/>
       <c r="L54" s="56"/>
-      <c r="M54" s="170"/>
+      <c r="M54" s="180"/>
       <c r="N54" s="103"/>
       <c r="O54" s="7"/>
       <c r="P54" s="7"/>
@@ -32561,11 +32567,11 @@
       <c r="Z54" s="7"/>
     </row>
     <row r="55" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A55" s="170"/>
-      <c r="B55" s="174"/>
-      <c r="C55" s="170"/>
+      <c r="A55" s="180"/>
+      <c r="B55" s="186"/>
+      <c r="C55" s="180"/>
       <c r="D55" s="57"/>
-      <c r="E55" s="170"/>
+      <c r="E55" s="180"/>
       <c r="F55" s="105" t="s">
         <v>157</v>
       </c>
@@ -32581,7 +32587,7 @@
       </c>
       <c r="K55" s="57"/>
       <c r="L55" s="56"/>
-      <c r="M55" s="170"/>
+      <c r="M55" s="180"/>
       <c r="N55" s="103"/>
       <c r="O55" s="7"/>
       <c r="P55" s="7"/>
@@ -32597,11 +32603,11 @@
       <c r="Z55" s="7"/>
     </row>
     <row r="56" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A56" s="170"/>
-      <c r="B56" s="174"/>
-      <c r="C56" s="170"/>
+      <c r="A56" s="180"/>
+      <c r="B56" s="186"/>
+      <c r="C56" s="180"/>
       <c r="D56" s="57"/>
-      <c r="E56" s="170"/>
+      <c r="E56" s="180"/>
       <c r="F56" s="105" t="s">
         <v>158</v>
       </c>
@@ -32617,7 +32623,7 @@
       </c>
       <c r="K56" s="57"/>
       <c r="L56" s="56"/>
-      <c r="M56" s="170"/>
+      <c r="M56" s="180"/>
       <c r="N56" s="103"/>
       <c r="O56" s="7"/>
       <c r="P56" s="7"/>
@@ -32633,11 +32639,11 @@
       <c r="Z56" s="7"/>
     </row>
     <row r="57" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A57" s="170"/>
-      <c r="B57" s="174"/>
-      <c r="C57" s="170"/>
+      <c r="A57" s="180"/>
+      <c r="B57" s="186"/>
+      <c r="C57" s="180"/>
       <c r="D57" s="57"/>
-      <c r="E57" s="170"/>
+      <c r="E57" s="180"/>
       <c r="F57" s="105" t="s">
         <v>162</v>
       </c>
@@ -32653,7 +32659,7 @@
       </c>
       <c r="K57" s="57"/>
       <c r="L57" s="56"/>
-      <c r="M57" s="170"/>
+      <c r="M57" s="180"/>
       <c r="N57" s="103"/>
       <c r="O57" s="7"/>
       <c r="P57" s="7"/>
@@ -32669,11 +32675,11 @@
       <c r="Z57" s="7"/>
     </row>
     <row r="58" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A58" s="170"/>
-      <c r="B58" s="174"/>
-      <c r="C58" s="170"/>
+      <c r="A58" s="180"/>
+      <c r="B58" s="186"/>
+      <c r="C58" s="180"/>
       <c r="D58" s="57"/>
-      <c r="E58" s="170"/>
+      <c r="E58" s="180"/>
       <c r="F58" s="105" t="s">
         <v>167</v>
       </c>
@@ -32689,7 +32695,7 @@
       </c>
       <c r="K58" s="57"/>
       <c r="L58" s="56"/>
-      <c r="M58" s="170"/>
+      <c r="M58" s="180"/>
       <c r="N58" s="103"/>
       <c r="O58" s="7"/>
       <c r="P58" s="7"/>
@@ -32705,11 +32711,11 @@
       <c r="Z58" s="7"/>
     </row>
     <row r="59" spans="1:26" ht="60" customHeight="1">
-      <c r="A59" s="170"/>
-      <c r="B59" s="174"/>
-      <c r="C59" s="170"/>
+      <c r="A59" s="180"/>
+      <c r="B59" s="186"/>
+      <c r="C59" s="180"/>
       <c r="D59" s="57"/>
-      <c r="E59" s="170"/>
+      <c r="E59" s="180"/>
       <c r="F59" s="105" t="s">
         <v>172</v>
       </c>
@@ -32725,7 +32731,7 @@
       </c>
       <c r="K59" s="57"/>
       <c r="L59" s="56"/>
-      <c r="M59" s="170"/>
+      <c r="M59" s="180"/>
       <c r="N59" s="103"/>
       <c r="O59" s="7"/>
       <c r="P59" s="7"/>
@@ -32741,11 +32747,11 @@
       <c r="Z59" s="7"/>
     </row>
     <row r="60" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A60" s="170"/>
-      <c r="B60" s="174"/>
-      <c r="C60" s="170"/>
+      <c r="A60" s="180"/>
+      <c r="B60" s="186"/>
+      <c r="C60" s="180"/>
       <c r="D60" s="57"/>
-      <c r="E60" s="170"/>
+      <c r="E60" s="180"/>
       <c r="F60" s="105" t="s">
         <v>173</v>
       </c>
@@ -32761,7 +32767,7 @@
       </c>
       <c r="K60" s="57"/>
       <c r="L60" s="56"/>
-      <c r="M60" s="170"/>
+      <c r="M60" s="180"/>
       <c r="N60" s="103"/>
       <c r="O60" s="7"/>
       <c r="P60" s="7"/>
@@ -32777,11 +32783,11 @@
       <c r="Z60" s="7"/>
     </row>
     <row r="61" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A61" s="170"/>
-      <c r="B61" s="174"/>
-      <c r="C61" s="170"/>
+      <c r="A61" s="180"/>
+      <c r="B61" s="186"/>
+      <c r="C61" s="180"/>
       <c r="D61" s="67"/>
-      <c r="E61" s="170"/>
+      <c r="E61" s="180"/>
       <c r="F61" s="93" t="s">
         <v>177</v>
       </c>
@@ -32797,7 +32803,7 @@
       </c>
       <c r="K61" s="67"/>
       <c r="L61" s="75"/>
-      <c r="M61" s="170"/>
+      <c r="M61" s="180"/>
       <c r="N61" s="104"/>
       <c r="O61" s="7"/>
       <c r="P61" s="7"/>
@@ -32813,17 +32819,17 @@
       <c r="Z61" s="7"/>
     </row>
     <row r="62" spans="1:26" ht="45.75" customHeight="1">
-      <c r="A62" s="171" t="s">
+      <c r="A62" s="181" t="s">
         <v>267</v>
       </c>
-      <c r="B62" s="173" t="s">
+      <c r="B62" s="184" t="s">
         <v>534</v>
       </c>
-      <c r="C62" s="171" t="s">
+      <c r="C62" s="181" t="s">
         <v>536</v>
       </c>
       <c r="D62" s="85"/>
-      <c r="E62" s="171" t="s">
+      <c r="E62" s="181" t="s">
         <v>537</v>
       </c>
       <c r="F62" s="46" t="s">
@@ -32859,11 +32865,11 @@
       <c r="Z62" s="7"/>
     </row>
     <row r="63" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A63" s="170"/>
-      <c r="B63" s="174"/>
-      <c r="C63" s="170"/>
+      <c r="A63" s="180"/>
+      <c r="B63" s="186"/>
+      <c r="C63" s="180"/>
       <c r="D63" s="57"/>
-      <c r="E63" s="170"/>
+      <c r="E63" s="180"/>
       <c r="F63" s="53" t="s">
         <v>182</v>
       </c>
@@ -32879,7 +32885,7 @@
       </c>
       <c r="K63" s="57"/>
       <c r="L63" s="56"/>
-      <c r="M63" s="171" t="s">
+      <c r="M63" s="181" t="s">
         <v>537</v>
       </c>
       <c r="N63" s="103"/>
@@ -32897,11 +32903,11 @@
       <c r="Z63" s="7"/>
     </row>
     <row r="64" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A64" s="170"/>
-      <c r="B64" s="174"/>
-      <c r="C64" s="170"/>
+      <c r="A64" s="180"/>
+      <c r="B64" s="186"/>
+      <c r="C64" s="180"/>
       <c r="D64" s="57"/>
-      <c r="E64" s="170"/>
+      <c r="E64" s="180"/>
       <c r="F64" s="53" t="s">
         <v>185</v>
       </c>
@@ -32917,7 +32923,7 @@
       </c>
       <c r="K64" s="57"/>
       <c r="L64" s="56"/>
-      <c r="M64" s="170"/>
+      <c r="M64" s="180"/>
       <c r="N64" s="103"/>
       <c r="O64" s="7"/>
       <c r="P64" s="7"/>
@@ -32933,11 +32939,11 @@
       <c r="Z64" s="7"/>
     </row>
     <row r="65" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A65" s="170"/>
-      <c r="B65" s="174"/>
-      <c r="C65" s="170"/>
+      <c r="A65" s="180"/>
+      <c r="B65" s="186"/>
+      <c r="C65" s="180"/>
       <c r="D65" s="57"/>
-      <c r="E65" s="170"/>
+      <c r="E65" s="180"/>
       <c r="F65" s="53" t="s">
         <v>188</v>
       </c>
@@ -32953,7 +32959,7 @@
       </c>
       <c r="K65" s="57"/>
       <c r="L65" s="56"/>
-      <c r="M65" s="170"/>
+      <c r="M65" s="180"/>
       <c r="N65" s="103"/>
       <c r="O65" s="7"/>
       <c r="P65" s="7"/>
@@ -32969,11 +32975,11 @@
       <c r="Z65" s="7"/>
     </row>
     <row r="66" spans="1:26" ht="96" customHeight="1">
-      <c r="A66" s="170"/>
-      <c r="B66" s="174"/>
-      <c r="C66" s="170"/>
+      <c r="A66" s="180"/>
+      <c r="B66" s="186"/>
+      <c r="C66" s="180"/>
       <c r="D66" s="57"/>
-      <c r="E66" s="170"/>
+      <c r="E66" s="180"/>
       <c r="F66" s="53" t="s">
         <v>189</v>
       </c>
@@ -32989,7 +32995,7 @@
       </c>
       <c r="K66" s="57"/>
       <c r="L66" s="56"/>
-      <c r="M66" s="170"/>
+      <c r="M66" s="180"/>
       <c r="N66" s="103"/>
       <c r="O66" s="7"/>
       <c r="P66" s="7"/>
@@ -33005,11 +33011,11 @@
       <c r="Z66" s="7"/>
     </row>
     <row r="67" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A67" s="170"/>
-      <c r="B67" s="174"/>
-      <c r="C67" s="170"/>
+      <c r="A67" s="180"/>
+      <c r="B67" s="186"/>
+      <c r="C67" s="180"/>
       <c r="D67" s="57"/>
-      <c r="E67" s="170"/>
+      <c r="E67" s="180"/>
       <c r="F67" s="53" t="s">
         <v>192</v>
       </c>
@@ -33025,7 +33031,7 @@
       </c>
       <c r="K67" s="57"/>
       <c r="L67" s="56"/>
-      <c r="M67" s="170"/>
+      <c r="M67" s="180"/>
       <c r="N67" s="103"/>
       <c r="O67" s="7"/>
       <c r="P67" s="7"/>
@@ -33041,11 +33047,11 @@
       <c r="Z67" s="7"/>
     </row>
     <row r="68" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A68" s="170"/>
-      <c r="B68" s="174"/>
-      <c r="C68" s="170"/>
+      <c r="A68" s="180"/>
+      <c r="B68" s="186"/>
+      <c r="C68" s="180"/>
       <c r="D68" s="57"/>
-      <c r="E68" s="170"/>
+      <c r="E68" s="180"/>
       <c r="F68" s="53" t="s">
         <v>198</v>
       </c>
@@ -33061,7 +33067,7 @@
       </c>
       <c r="K68" s="57"/>
       <c r="L68" s="56"/>
-      <c r="M68" s="170"/>
+      <c r="M68" s="180"/>
       <c r="N68" s="103"/>
       <c r="O68" s="7"/>
       <c r="P68" s="7"/>
@@ -33077,11 +33083,11 @@
       <c r="Z68" s="7"/>
     </row>
     <row r="69" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A69" s="170"/>
-      <c r="B69" s="174"/>
-      <c r="C69" s="170"/>
+      <c r="A69" s="180"/>
+      <c r="B69" s="186"/>
+      <c r="C69" s="180"/>
       <c r="D69" s="57"/>
-      <c r="E69" s="170"/>
+      <c r="E69" s="180"/>
       <c r="F69" s="53" t="s">
         <v>201</v>
       </c>
@@ -33097,7 +33103,7 @@
       </c>
       <c r="K69" s="57"/>
       <c r="L69" s="56"/>
-      <c r="M69" s="170"/>
+      <c r="M69" s="180"/>
       <c r="N69" s="103"/>
       <c r="O69" s="7"/>
       <c r="P69" s="7"/>
@@ -33113,11 +33119,11 @@
       <c r="Z69" s="7"/>
     </row>
     <row r="70" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A70" s="170"/>
-      <c r="B70" s="174"/>
-      <c r="C70" s="170"/>
+      <c r="A70" s="180"/>
+      <c r="B70" s="186"/>
+      <c r="C70" s="180"/>
       <c r="D70" s="57"/>
-      <c r="E70" s="170"/>
+      <c r="E70" s="180"/>
       <c r="F70" s="53" t="s">
         <v>207</v>
       </c>
@@ -33133,7 +33139,7 @@
       </c>
       <c r="K70" s="57"/>
       <c r="L70" s="56"/>
-      <c r="M70" s="170"/>
+      <c r="M70" s="180"/>
       <c r="N70" s="103"/>
       <c r="O70" s="7"/>
       <c r="P70" s="7"/>
@@ -33149,11 +33155,11 @@
       <c r="Z70" s="7"/>
     </row>
     <row r="71" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A71" s="170"/>
-      <c r="B71" s="174"/>
-      <c r="C71" s="170"/>
+      <c r="A71" s="180"/>
+      <c r="B71" s="186"/>
+      <c r="C71" s="180"/>
       <c r="D71" s="57"/>
-      <c r="E71" s="170"/>
+      <c r="E71" s="180"/>
       <c r="F71" s="53" t="s">
         <v>208</v>
       </c>
@@ -33169,7 +33175,7 @@
       </c>
       <c r="K71" s="57"/>
       <c r="L71" s="56"/>
-      <c r="M71" s="170"/>
+      <c r="M71" s="180"/>
       <c r="N71" s="103"/>
       <c r="O71" s="7"/>
       <c r="P71" s="7"/>
@@ -33185,11 +33191,11 @@
       <c r="Z71" s="7"/>
     </row>
     <row r="72" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A72" s="170"/>
-      <c r="B72" s="174"/>
-      <c r="C72" s="170"/>
+      <c r="A72" s="180"/>
+      <c r="B72" s="186"/>
+      <c r="C72" s="180"/>
       <c r="D72" s="57"/>
-      <c r="E72" s="170"/>
+      <c r="E72" s="180"/>
       <c r="F72" s="53" t="s">
         <v>210</v>
       </c>
@@ -33205,7 +33211,7 @@
       </c>
       <c r="K72" s="57"/>
       <c r="L72" s="56"/>
-      <c r="M72" s="170"/>
+      <c r="M72" s="180"/>
       <c r="N72" s="103"/>
       <c r="O72" s="7"/>
       <c r="P72" s="7"/>
@@ -33221,11 +33227,11 @@
       <c r="Z72" s="7"/>
     </row>
     <row r="73" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A73" s="170"/>
-      <c r="B73" s="174"/>
-      <c r="C73" s="170"/>
+      <c r="A73" s="180"/>
+      <c r="B73" s="186"/>
+      <c r="C73" s="180"/>
       <c r="D73" s="57"/>
-      <c r="E73" s="170"/>
+      <c r="E73" s="180"/>
       <c r="F73" s="53" t="s">
         <v>211</v>
       </c>
@@ -33241,7 +33247,7 @@
       </c>
       <c r="K73" s="57"/>
       <c r="L73" s="56"/>
-      <c r="M73" s="170"/>
+      <c r="M73" s="180"/>
       <c r="N73" s="103"/>
       <c r="O73" s="7"/>
       <c r="P73" s="7"/>
@@ -33257,11 +33263,11 @@
       <c r="Z73" s="7"/>
     </row>
     <row r="74" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A74" s="170"/>
-      <c r="B74" s="174"/>
-      <c r="C74" s="170"/>
+      <c r="A74" s="180"/>
+      <c r="B74" s="186"/>
+      <c r="C74" s="180"/>
       <c r="D74" s="57"/>
-      <c r="E74" s="170"/>
+      <c r="E74" s="180"/>
       <c r="F74" s="53" t="s">
         <v>214</v>
       </c>
@@ -33277,7 +33283,7 @@
       </c>
       <c r="K74" s="57"/>
       <c r="L74" s="56"/>
-      <c r="M74" s="170"/>
+      <c r="M74" s="180"/>
       <c r="N74" s="103"/>
       <c r="O74" s="7"/>
       <c r="P74" s="7"/>
@@ -33293,11 +33299,11 @@
       <c r="Z74" s="7"/>
     </row>
     <row r="75" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A75" s="172"/>
-      <c r="B75" s="175"/>
-      <c r="C75" s="172"/>
+      <c r="A75" s="182"/>
+      <c r="B75" s="185"/>
+      <c r="C75" s="182"/>
       <c r="D75" s="94"/>
-      <c r="E75" s="172"/>
+      <c r="E75" s="182"/>
       <c r="F75" s="63" t="s">
         <v>217</v>
       </c>
@@ -33313,7 +33319,7 @@
       </c>
       <c r="K75" s="94"/>
       <c r="L75" s="89"/>
-      <c r="M75" s="172"/>
+      <c r="M75" s="182"/>
       <c r="N75" s="106"/>
       <c r="O75" s="7"/>
       <c r="P75" s="7"/>
@@ -33329,17 +33335,17 @@
       <c r="Z75" s="7"/>
     </row>
     <row r="76" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A76" s="171" t="s">
+      <c r="A76" s="181" t="s">
         <v>291</v>
       </c>
-      <c r="B76" s="173" t="s">
+      <c r="B76" s="184" t="s">
         <v>551</v>
       </c>
-      <c r="C76" s="171" t="s">
+      <c r="C76" s="181" t="s">
         <v>552</v>
       </c>
       <c r="D76" s="85"/>
-      <c r="E76" s="171" t="s">
+      <c r="E76" s="181" t="s">
         <v>553</v>
       </c>
       <c r="F76" s="46" t="s">
@@ -33357,7 +33363,7 @@
       </c>
       <c r="K76" s="85"/>
       <c r="L76" s="86"/>
-      <c r="M76" s="171" t="s">
+      <c r="M76" s="181" t="s">
         <v>556</v>
       </c>
       <c r="N76" s="102"/>
@@ -33375,11 +33381,11 @@
       <c r="Z76" s="7"/>
     </row>
     <row r="77" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A77" s="170"/>
-      <c r="B77" s="174"/>
-      <c r="C77" s="170"/>
+      <c r="A77" s="180"/>
+      <c r="B77" s="186"/>
+      <c r="C77" s="180"/>
       <c r="D77" s="57"/>
-      <c r="E77" s="170"/>
+      <c r="E77" s="180"/>
       <c r="F77" s="53" t="s">
         <v>224</v>
       </c>
@@ -33395,7 +33401,7 @@
       </c>
       <c r="K77" s="57"/>
       <c r="L77" s="56"/>
-      <c r="M77" s="170"/>
+      <c r="M77" s="180"/>
       <c r="N77" s="103"/>
       <c r="O77" s="7"/>
       <c r="P77" s="7"/>
@@ -33411,11 +33417,11 @@
       <c r="Z77" s="7"/>
     </row>
     <row r="78" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A78" s="170"/>
-      <c r="B78" s="174"/>
-      <c r="C78" s="170"/>
+      <c r="A78" s="180"/>
+      <c r="B78" s="186"/>
+      <c r="C78" s="180"/>
       <c r="D78" s="57"/>
-      <c r="E78" s="170"/>
+      <c r="E78" s="180"/>
       <c r="F78" s="70" t="s">
         <v>231</v>
       </c>
@@ -33431,7 +33437,7 @@
       </c>
       <c r="K78" s="57"/>
       <c r="L78" s="56"/>
-      <c r="M78" s="170"/>
+      <c r="M78" s="180"/>
       <c r="N78" s="103"/>
       <c r="O78" s="7"/>
       <c r="P78" s="7"/>
@@ -33447,11 +33453,11 @@
       <c r="Z78" s="7"/>
     </row>
     <row r="79" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A79" s="170"/>
-      <c r="B79" s="174"/>
-      <c r="C79" s="170"/>
+      <c r="A79" s="180"/>
+      <c r="B79" s="186"/>
+      <c r="C79" s="180"/>
       <c r="D79" s="57"/>
-      <c r="E79" s="170"/>
+      <c r="E79" s="180"/>
       <c r="F79" s="53" t="s">
         <v>233</v>
       </c>
@@ -33467,7 +33473,7 @@
       </c>
       <c r="K79" s="57"/>
       <c r="L79" s="56"/>
-      <c r="M79" s="170"/>
+      <c r="M79" s="180"/>
       <c r="N79" s="103"/>
       <c r="O79" s="7"/>
       <c r="P79" s="7"/>
@@ -33483,11 +33489,11 @@
       <c r="Z79" s="7"/>
     </row>
     <row r="80" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A80" s="170"/>
-      <c r="B80" s="174"/>
-      <c r="C80" s="170"/>
+      <c r="A80" s="180"/>
+      <c r="B80" s="186"/>
+      <c r="C80" s="180"/>
       <c r="D80" s="57"/>
-      <c r="E80" s="170"/>
+      <c r="E80" s="180"/>
       <c r="F80" s="53" t="s">
         <v>238</v>
       </c>
@@ -33503,7 +33509,7 @@
       </c>
       <c r="K80" s="57"/>
       <c r="L80" s="56"/>
-      <c r="M80" s="170"/>
+      <c r="M80" s="180"/>
       <c r="N80" s="103"/>
       <c r="O80" s="7"/>
       <c r="P80" s="7"/>
@@ -33519,11 +33525,11 @@
       <c r="Z80" s="7"/>
     </row>
     <row r="81" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A81" s="170"/>
-      <c r="B81" s="174"/>
-      <c r="C81" s="170"/>
+      <c r="A81" s="180"/>
+      <c r="B81" s="186"/>
+      <c r="C81" s="180"/>
       <c r="D81" s="57"/>
-      <c r="E81" s="170"/>
+      <c r="E81" s="180"/>
       <c r="F81" s="70" t="s">
         <v>239</v>
       </c>
@@ -33539,7 +33545,7 @@
       </c>
       <c r="K81" s="57"/>
       <c r="L81" s="56"/>
-      <c r="M81" s="170"/>
+      <c r="M81" s="180"/>
       <c r="N81" s="103"/>
       <c r="O81" s="7"/>
       <c r="P81" s="7"/>
@@ -33555,11 +33561,11 @@
       <c r="Z81" s="7"/>
     </row>
     <row r="82" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A82" s="170"/>
-      <c r="B82" s="174"/>
-      <c r="C82" s="170"/>
+      <c r="A82" s="180"/>
+      <c r="B82" s="186"/>
+      <c r="C82" s="180"/>
       <c r="D82" s="57"/>
-      <c r="E82" s="170"/>
+      <c r="E82" s="180"/>
       <c r="F82" s="53" t="s">
         <v>242</v>
       </c>
@@ -33575,7 +33581,7 @@
       </c>
       <c r="K82" s="57"/>
       <c r="L82" s="56"/>
-      <c r="M82" s="170"/>
+      <c r="M82" s="180"/>
       <c r="N82" s="103"/>
       <c r="O82" s="7"/>
       <c r="P82" s="7"/>
@@ -33591,11 +33597,11 @@
       <c r="Z82" s="7"/>
     </row>
     <row r="83" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A83" s="170"/>
-      <c r="B83" s="174"/>
-      <c r="C83" s="170"/>
+      <c r="A83" s="180"/>
+      <c r="B83" s="186"/>
+      <c r="C83" s="180"/>
       <c r="D83" s="57"/>
-      <c r="E83" s="170"/>
+      <c r="E83" s="180"/>
       <c r="F83" s="53" t="s">
         <v>245</v>
       </c>
@@ -33611,7 +33617,7 @@
       </c>
       <c r="K83" s="57"/>
       <c r="L83" s="56"/>
-      <c r="M83" s="170"/>
+      <c r="M83" s="180"/>
       <c r="N83" s="103"/>
       <c r="O83" s="7"/>
       <c r="P83" s="7"/>
@@ -33627,11 +33633,11 @@
       <c r="Z83" s="7"/>
     </row>
     <row r="84" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A84" s="170"/>
-      <c r="B84" s="174"/>
-      <c r="C84" s="170"/>
+      <c r="A84" s="180"/>
+      <c r="B84" s="186"/>
+      <c r="C84" s="180"/>
       <c r="D84" s="57"/>
-      <c r="E84" s="170"/>
+      <c r="E84" s="180"/>
       <c r="F84" s="70" t="s">
         <v>248</v>
       </c>
@@ -33647,7 +33653,7 @@
       </c>
       <c r="K84" s="57"/>
       <c r="L84" s="56"/>
-      <c r="M84" s="170"/>
+      <c r="M84" s="180"/>
       <c r="N84" s="103"/>
       <c r="O84" s="7"/>
       <c r="P84" s="7"/>
@@ -33663,11 +33669,11 @@
       <c r="Z84" s="7"/>
     </row>
     <row r="85" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A85" s="170"/>
-      <c r="B85" s="174"/>
-      <c r="C85" s="170"/>
+      <c r="A85" s="180"/>
+      <c r="B85" s="186"/>
+      <c r="C85" s="180"/>
       <c r="D85" s="57"/>
-      <c r="E85" s="170"/>
+      <c r="E85" s="180"/>
       <c r="F85" s="53" t="s">
         <v>252</v>
       </c>
@@ -33683,7 +33689,7 @@
       </c>
       <c r="K85" s="57"/>
       <c r="L85" s="56"/>
-      <c r="M85" s="170"/>
+      <c r="M85" s="180"/>
       <c r="N85" s="103"/>
       <c r="O85" s="7"/>
       <c r="P85" s="7"/>
@@ -33699,11 +33705,11 @@
       <c r="Z85" s="7"/>
     </row>
     <row r="86" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A86" s="170"/>
-      <c r="B86" s="174"/>
-      <c r="C86" s="170"/>
+      <c r="A86" s="180"/>
+      <c r="B86" s="186"/>
+      <c r="C86" s="180"/>
       <c r="D86" s="57"/>
-      <c r="E86" s="170"/>
+      <c r="E86" s="180"/>
       <c r="F86" s="53" t="s">
         <v>259</v>
       </c>
@@ -33719,7 +33725,7 @@
       </c>
       <c r="K86" s="57"/>
       <c r="L86" s="56"/>
-      <c r="M86" s="159"/>
+      <c r="M86" s="169"/>
       <c r="N86" s="103"/>
       <c r="O86" s="7"/>
       <c r="P86" s="7"/>
@@ -33735,11 +33741,11 @@
       <c r="Z86" s="7"/>
     </row>
     <row r="87" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A87" s="170"/>
-      <c r="B87" s="181"/>
-      <c r="C87" s="159"/>
+      <c r="A87" s="180"/>
+      <c r="B87" s="196"/>
+      <c r="C87" s="169"/>
       <c r="D87" s="67"/>
-      <c r="E87" s="170"/>
+      <c r="E87" s="180"/>
       <c r="F87" s="70" t="s">
         <v>260</v>
       </c>
@@ -33773,17 +33779,17 @@
       <c r="Z87" s="7"/>
     </row>
     <row r="88" spans="1:26" ht="30" customHeight="1">
-      <c r="A88" s="171" t="s">
+      <c r="A88" s="181" t="s">
         <v>345</v>
       </c>
-      <c r="B88" s="173" t="s">
+      <c r="B88" s="184" t="s">
         <v>576</v>
       </c>
-      <c r="C88" s="171" t="s">
+      <c r="C88" s="181" t="s">
         <v>577</v>
       </c>
       <c r="D88" s="85"/>
-      <c r="E88" s="171" t="s">
+      <c r="E88" s="181" t="s">
         <v>578</v>
       </c>
       <c r="F88" s="46" t="s">
@@ -33801,7 +33807,7 @@
       </c>
       <c r="K88" s="85"/>
       <c r="L88" s="86"/>
-      <c r="M88" s="171" t="s">
+      <c r="M88" s="181" t="s">
         <v>578</v>
       </c>
       <c r="N88" s="102"/>
@@ -33819,11 +33825,11 @@
       <c r="Z88" s="7"/>
     </row>
     <row r="89" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A89" s="170"/>
-      <c r="B89" s="174"/>
-      <c r="C89" s="170"/>
+      <c r="A89" s="180"/>
+      <c r="B89" s="186"/>
+      <c r="C89" s="180"/>
       <c r="D89" s="57"/>
-      <c r="E89" s="170"/>
+      <c r="E89" s="180"/>
       <c r="F89" s="53" t="s">
         <v>262</v>
       </c>
@@ -33839,7 +33845,7 @@
       </c>
       <c r="K89" s="57"/>
       <c r="L89" s="56"/>
-      <c r="M89" s="170"/>
+      <c r="M89" s="180"/>
       <c r="N89" s="103"/>
       <c r="O89" s="7"/>
       <c r="P89" s="7"/>
@@ -33855,11 +33861,11 @@
       <c r="Z89" s="7"/>
     </row>
     <row r="90" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A90" s="170"/>
-      <c r="B90" s="174"/>
-      <c r="C90" s="170"/>
+      <c r="A90" s="180"/>
+      <c r="B90" s="186"/>
+      <c r="C90" s="180"/>
       <c r="D90" s="57"/>
-      <c r="E90" s="170"/>
+      <c r="E90" s="180"/>
       <c r="F90" s="53" t="s">
         <v>275</v>
       </c>
@@ -33875,7 +33881,7 @@
       </c>
       <c r="K90" s="57"/>
       <c r="L90" s="56"/>
-      <c r="M90" s="170"/>
+      <c r="M90" s="180"/>
       <c r="N90" s="103"/>
       <c r="O90" s="7"/>
       <c r="P90" s="7"/>
@@ -33891,11 +33897,11 @@
       <c r="Z90" s="7"/>
     </row>
     <row r="91" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A91" s="170"/>
-      <c r="B91" s="174"/>
-      <c r="C91" s="170"/>
+      <c r="A91" s="180"/>
+      <c r="B91" s="186"/>
+      <c r="C91" s="180"/>
       <c r="D91" s="57"/>
-      <c r="E91" s="170"/>
+      <c r="E91" s="180"/>
       <c r="F91" s="53" t="s">
         <v>283</v>
       </c>
@@ -33911,7 +33917,7 @@
       </c>
       <c r="K91" s="57"/>
       <c r="L91" s="56"/>
-      <c r="M91" s="170"/>
+      <c r="M91" s="180"/>
       <c r="N91" s="103"/>
       <c r="O91" s="7"/>
       <c r="P91" s="7"/>
@@ -33927,11 +33933,11 @@
       <c r="Z91" s="7"/>
     </row>
     <row r="92" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A92" s="170"/>
-      <c r="B92" s="174"/>
-      <c r="C92" s="170"/>
+      <c r="A92" s="180"/>
+      <c r="B92" s="186"/>
+      <c r="C92" s="180"/>
       <c r="D92" s="57"/>
-      <c r="E92" s="170"/>
+      <c r="E92" s="180"/>
       <c r="F92" s="53" t="s">
         <v>286</v>
       </c>
@@ -33947,7 +33953,7 @@
       </c>
       <c r="K92" s="57"/>
       <c r="L92" s="56"/>
-      <c r="M92" s="170"/>
+      <c r="M92" s="180"/>
       <c r="N92" s="103"/>
       <c r="O92" s="7"/>
       <c r="P92" s="7"/>
@@ -33963,11 +33969,11 @@
       <c r="Z92" s="7"/>
     </row>
     <row r="93" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A93" s="170"/>
-      <c r="B93" s="174"/>
-      <c r="C93" s="170"/>
+      <c r="A93" s="180"/>
+      <c r="B93" s="186"/>
+      <c r="C93" s="180"/>
       <c r="D93" s="57"/>
-      <c r="E93" s="170"/>
+      <c r="E93" s="180"/>
       <c r="F93" s="53" t="s">
         <v>288</v>
       </c>
@@ -33983,7 +33989,7 @@
       </c>
       <c r="K93" s="57"/>
       <c r="L93" s="56"/>
-      <c r="M93" s="170"/>
+      <c r="M93" s="180"/>
       <c r="N93" s="103"/>
       <c r="O93" s="7"/>
       <c r="P93" s="7"/>
@@ -33999,11 +34005,11 @@
       <c r="Z93" s="7"/>
     </row>
     <row r="94" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A94" s="170"/>
-      <c r="B94" s="174"/>
-      <c r="C94" s="170"/>
+      <c r="A94" s="180"/>
+      <c r="B94" s="186"/>
+      <c r="C94" s="180"/>
       <c r="D94" s="57"/>
-      <c r="E94" s="170"/>
+      <c r="E94" s="180"/>
       <c r="F94" s="53" t="s">
         <v>295</v>
       </c>
@@ -34019,7 +34025,7 @@
       </c>
       <c r="K94" s="57"/>
       <c r="L94" s="56"/>
-      <c r="M94" s="170"/>
+      <c r="M94" s="180"/>
       <c r="N94" s="103"/>
       <c r="O94" s="7"/>
       <c r="P94" s="7"/>
@@ -34035,11 +34041,11 @@
       <c r="Z94" s="7"/>
     </row>
     <row r="95" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A95" s="170"/>
-      <c r="B95" s="174"/>
-      <c r="C95" s="170"/>
+      <c r="A95" s="180"/>
+      <c r="B95" s="186"/>
+      <c r="C95" s="180"/>
       <c r="D95" s="57"/>
-      <c r="E95" s="170"/>
+      <c r="E95" s="180"/>
       <c r="F95" s="53" t="s">
         <v>302</v>
       </c>
@@ -34055,7 +34061,7 @@
       </c>
       <c r="K95" s="57"/>
       <c r="L95" s="56"/>
-      <c r="M95" s="170"/>
+      <c r="M95" s="180"/>
       <c r="N95" s="103"/>
       <c r="O95" s="7"/>
       <c r="P95" s="7"/>
@@ -34071,11 +34077,11 @@
       <c r="Z95" s="7"/>
     </row>
     <row r="96" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A96" s="170"/>
-      <c r="B96" s="174"/>
-      <c r="C96" s="170"/>
+      <c r="A96" s="180"/>
+      <c r="B96" s="186"/>
+      <c r="C96" s="180"/>
       <c r="D96" s="57"/>
-      <c r="E96" s="170"/>
+      <c r="E96" s="180"/>
       <c r="F96" s="53" t="s">
         <v>305</v>
       </c>
@@ -34091,7 +34097,7 @@
       </c>
       <c r="K96" s="57"/>
       <c r="L96" s="56"/>
-      <c r="M96" s="170"/>
+      <c r="M96" s="180"/>
       <c r="N96" s="103"/>
       <c r="O96" s="7"/>
       <c r="P96" s="7"/>
@@ -34107,11 +34113,11 @@
       <c r="Z96" s="7"/>
     </row>
     <row r="97" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A97" s="170"/>
-      <c r="B97" s="174"/>
-      <c r="C97" s="170"/>
+      <c r="A97" s="180"/>
+      <c r="B97" s="186"/>
+      <c r="C97" s="180"/>
       <c r="D97" s="57"/>
-      <c r="E97" s="170"/>
+      <c r="E97" s="180"/>
       <c r="F97" s="53" t="s">
         <v>310</v>
       </c>
@@ -34127,7 +34133,7 @@
       </c>
       <c r="K97" s="57"/>
       <c r="L97" s="56"/>
-      <c r="M97" s="170"/>
+      <c r="M97" s="180"/>
       <c r="N97" s="103"/>
       <c r="O97" s="7"/>
       <c r="P97" s="7"/>
@@ -34143,11 +34149,11 @@
       <c r="Z97" s="7"/>
     </row>
     <row r="98" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A98" s="170"/>
-      <c r="B98" s="174"/>
-      <c r="C98" s="170"/>
+      <c r="A98" s="180"/>
+      <c r="B98" s="186"/>
+      <c r="C98" s="180"/>
       <c r="D98" s="57"/>
-      <c r="E98" s="170"/>
+      <c r="E98" s="180"/>
       <c r="F98" s="53" t="s">
         <v>315</v>
       </c>
@@ -34163,7 +34169,7 @@
       </c>
       <c r="K98" s="57"/>
       <c r="L98" s="56"/>
-      <c r="M98" s="170"/>
+      <c r="M98" s="180"/>
       <c r="N98" s="103"/>
       <c r="O98" s="7"/>
       <c r="P98" s="7"/>
@@ -34179,11 +34185,11 @@
       <c r="Z98" s="7"/>
     </row>
     <row r="99" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A99" s="170"/>
-      <c r="B99" s="174"/>
-      <c r="C99" s="170"/>
+      <c r="A99" s="180"/>
+      <c r="B99" s="186"/>
+      <c r="C99" s="180"/>
       <c r="D99" s="57"/>
-      <c r="E99" s="170"/>
+      <c r="E99" s="180"/>
       <c r="F99" s="53" t="s">
         <v>319</v>
       </c>
@@ -34199,7 +34205,7 @@
       </c>
       <c r="K99" s="57"/>
       <c r="L99" s="56"/>
-      <c r="M99" s="170"/>
+      <c r="M99" s="180"/>
       <c r="N99" s="103"/>
       <c r="O99" s="7"/>
       <c r="P99" s="7"/>
@@ -34215,11 +34221,11 @@
       <c r="Z99" s="7"/>
     </row>
     <row r="100" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A100" s="170"/>
-      <c r="B100" s="174"/>
-      <c r="C100" s="170"/>
+      <c r="A100" s="180"/>
+      <c r="B100" s="186"/>
+      <c r="C100" s="180"/>
       <c r="D100" s="57"/>
-      <c r="E100" s="170"/>
+      <c r="E100" s="180"/>
       <c r="F100" s="53" t="s">
         <v>321</v>
       </c>
@@ -34235,7 +34241,7 @@
       </c>
       <c r="K100" s="57"/>
       <c r="L100" s="56"/>
-      <c r="M100" s="170"/>
+      <c r="M100" s="180"/>
       <c r="N100" s="103"/>
       <c r="O100" s="7"/>
       <c r="P100" s="7"/>
@@ -34251,11 +34257,11 @@
       <c r="Z100" s="7"/>
     </row>
     <row r="101" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A101" s="170"/>
-      <c r="B101" s="174"/>
-      <c r="C101" s="170"/>
+      <c r="A101" s="180"/>
+      <c r="B101" s="186"/>
+      <c r="C101" s="180"/>
       <c r="D101" s="57"/>
-      <c r="E101" s="170"/>
+      <c r="E101" s="180"/>
       <c r="F101" s="53" t="s">
         <v>324</v>
       </c>
@@ -34271,7 +34277,7 @@
       </c>
       <c r="K101" s="57"/>
       <c r="L101" s="56"/>
-      <c r="M101" s="170"/>
+      <c r="M101" s="180"/>
       <c r="N101" s="103"/>
       <c r="O101" s="7"/>
       <c r="P101" s="7"/>
@@ -34287,11 +34293,11 @@
       <c r="Z101" s="7"/>
     </row>
     <row r="102" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A102" s="170"/>
-      <c r="B102" s="174"/>
-      <c r="C102" s="170"/>
+      <c r="A102" s="180"/>
+      <c r="B102" s="186"/>
+      <c r="C102" s="180"/>
       <c r="D102" s="57"/>
-      <c r="E102" s="170"/>
+      <c r="E102" s="180"/>
       <c r="F102" s="53" t="s">
         <v>328</v>
       </c>
@@ -34307,7 +34313,7 @@
       </c>
       <c r="K102" s="57"/>
       <c r="L102" s="56"/>
-      <c r="M102" s="170"/>
+      <c r="M102" s="180"/>
       <c r="N102" s="103"/>
       <c r="O102" s="7"/>
       <c r="P102" s="7"/>
@@ -34323,11 +34329,11 @@
       <c r="Z102" s="7"/>
     </row>
     <row r="103" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A103" s="170"/>
-      <c r="B103" s="174"/>
-      <c r="C103" s="170"/>
+      <c r="A103" s="180"/>
+      <c r="B103" s="186"/>
+      <c r="C103" s="180"/>
       <c r="D103" s="57"/>
-      <c r="E103" s="170"/>
+      <c r="E103" s="180"/>
       <c r="F103" s="53" t="s">
         <v>330</v>
       </c>
@@ -34343,7 +34349,7 @@
       </c>
       <c r="K103" s="57"/>
       <c r="L103" s="56"/>
-      <c r="M103" s="170"/>
+      <c r="M103" s="180"/>
       <c r="N103" s="103"/>
       <c r="O103" s="7"/>
       <c r="P103" s="7"/>
@@ -34359,11 +34365,11 @@
       <c r="Z103" s="7"/>
     </row>
     <row r="104" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A104" s="170"/>
-      <c r="B104" s="174"/>
-      <c r="C104" s="170"/>
+      <c r="A104" s="180"/>
+      <c r="B104" s="186"/>
+      <c r="C104" s="180"/>
       <c r="D104" s="57"/>
-      <c r="E104" s="170"/>
+      <c r="E104" s="180"/>
       <c r="F104" s="53" t="s">
         <v>331</v>
       </c>
@@ -34397,11 +34403,11 @@
       <c r="Z104" s="7"/>
     </row>
     <row r="105" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A105" s="172"/>
-      <c r="B105" s="175"/>
-      <c r="C105" s="172"/>
+      <c r="A105" s="182"/>
+      <c r="B105" s="185"/>
+      <c r="C105" s="182"/>
       <c r="D105" s="94"/>
-      <c r="E105" s="172"/>
+      <c r="E105" s="182"/>
       <c r="F105" s="63" t="s">
         <v>337</v>
       </c>
@@ -34435,17 +34441,17 @@
       <c r="Z105" s="7"/>
     </row>
     <row r="106" spans="1:26" ht="15" customHeight="1">
-      <c r="A106" s="171" t="s">
+      <c r="A106" s="181" t="s">
         <v>376</v>
       </c>
-      <c r="B106" s="173" t="s">
+      <c r="B106" s="184" t="s">
         <v>612</v>
       </c>
-      <c r="C106" s="171" t="s">
+      <c r="C106" s="181" t="s">
         <v>613</v>
       </c>
       <c r="D106" s="85"/>
-      <c r="E106" s="171" t="s">
+      <c r="E106" s="181" t="s">
         <v>614</v>
       </c>
       <c r="F106" s="46" t="s">
@@ -34463,7 +34469,7 @@
       </c>
       <c r="K106" s="85"/>
       <c r="L106" s="86"/>
-      <c r="M106" s="171" t="s">
+      <c r="M106" s="181" t="s">
         <v>614</v>
       </c>
       <c r="N106" s="102"/>
@@ -34481,11 +34487,11 @@
       <c r="Z106" s="7"/>
     </row>
     <row r="107" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A107" s="170"/>
-      <c r="B107" s="174"/>
-      <c r="C107" s="170"/>
+      <c r="A107" s="180"/>
+      <c r="B107" s="186"/>
+      <c r="C107" s="180"/>
       <c r="D107" s="57"/>
-      <c r="E107" s="170"/>
+      <c r="E107" s="180"/>
       <c r="F107" s="53" t="s">
         <v>342</v>
       </c>
@@ -34501,7 +34507,7 @@
       </c>
       <c r="K107" s="57"/>
       <c r="L107" s="56"/>
-      <c r="M107" s="170"/>
+      <c r="M107" s="180"/>
       <c r="N107" s="103"/>
       <c r="O107" s="7"/>
       <c r="P107" s="7"/>
@@ -34517,11 +34523,11 @@
       <c r="Z107" s="7"/>
     </row>
     <row r="108" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A108" s="170"/>
-      <c r="B108" s="174"/>
-      <c r="C108" s="170"/>
+      <c r="A108" s="180"/>
+      <c r="B108" s="186"/>
+      <c r="C108" s="180"/>
       <c r="D108" s="57"/>
-      <c r="E108" s="170"/>
+      <c r="E108" s="180"/>
       <c r="F108" s="105" t="s">
         <v>348</v>
       </c>
@@ -34537,7 +34543,7 @@
       </c>
       <c r="K108" s="57"/>
       <c r="L108" s="56"/>
-      <c r="M108" s="170"/>
+      <c r="M108" s="180"/>
       <c r="N108" s="103"/>
       <c r="O108" s="7"/>
       <c r="P108" s="7"/>
@@ -34553,11 +34559,11 @@
       <c r="Z108" s="7"/>
     </row>
     <row r="109" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A109" s="170"/>
-      <c r="B109" s="174"/>
-      <c r="C109" s="170"/>
+      <c r="A109" s="180"/>
+      <c r="B109" s="186"/>
+      <c r="C109" s="180"/>
       <c r="D109" s="57"/>
-      <c r="E109" s="170"/>
+      <c r="E109" s="180"/>
       <c r="F109" s="53" t="s">
         <v>352</v>
       </c>
@@ -34573,7 +34579,7 @@
       </c>
       <c r="K109" s="57"/>
       <c r="L109" s="56"/>
-      <c r="M109" s="170"/>
+      <c r="M109" s="180"/>
       <c r="N109" s="103"/>
       <c r="O109" s="7"/>
       <c r="P109" s="7"/>
@@ -34589,11 +34595,11 @@
       <c r="Z109" s="7"/>
     </row>
     <row r="110" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A110" s="170"/>
-      <c r="B110" s="174"/>
-      <c r="C110" s="170"/>
+      <c r="A110" s="180"/>
+      <c r="B110" s="186"/>
+      <c r="C110" s="180"/>
       <c r="D110" s="57"/>
-      <c r="E110" s="170"/>
+      <c r="E110" s="180"/>
       <c r="F110" s="105" t="s">
         <v>361</v>
       </c>
@@ -34609,7 +34615,7 @@
       </c>
       <c r="K110" s="57"/>
       <c r="L110" s="56"/>
-      <c r="M110" s="170"/>
+      <c r="M110" s="180"/>
       <c r="N110" s="103"/>
       <c r="O110" s="7"/>
       <c r="P110" s="7"/>
@@ -34625,11 +34631,11 @@
       <c r="Z110" s="7"/>
     </row>
     <row r="111" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A111" s="170"/>
-      <c r="B111" s="174"/>
-      <c r="C111" s="170"/>
+      <c r="A111" s="180"/>
+      <c r="B111" s="186"/>
+      <c r="C111" s="180"/>
       <c r="D111" s="57"/>
-      <c r="E111" s="170"/>
+      <c r="E111" s="180"/>
       <c r="F111" s="53" t="s">
         <v>364</v>
       </c>
@@ -34645,7 +34651,7 @@
       </c>
       <c r="K111" s="57"/>
       <c r="L111" s="56"/>
-      <c r="M111" s="170"/>
+      <c r="M111" s="180"/>
       <c r="N111" s="103"/>
       <c r="O111" s="7"/>
       <c r="P111" s="7"/>
@@ -34661,11 +34667,11 @@
       <c r="Z111" s="7"/>
     </row>
     <row r="112" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A112" s="170"/>
-      <c r="B112" s="174"/>
-      <c r="C112" s="170"/>
+      <c r="A112" s="180"/>
+      <c r="B112" s="186"/>
+      <c r="C112" s="180"/>
       <c r="D112" s="57"/>
-      <c r="E112" s="170"/>
+      <c r="E112" s="180"/>
       <c r="F112" s="105" t="s">
         <v>369</v>
       </c>
@@ -34681,7 +34687,7 @@
       </c>
       <c r="K112" s="57"/>
       <c r="L112" s="56"/>
-      <c r="M112" s="159"/>
+      <c r="M112" s="169"/>
       <c r="N112" s="103"/>
       <c r="O112" s="7"/>
       <c r="P112" s="7"/>
@@ -34697,11 +34703,11 @@
       <c r="Z112" s="7"/>
     </row>
     <row r="113" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A113" s="172"/>
-      <c r="B113" s="175"/>
-      <c r="C113" s="172"/>
+      <c r="A113" s="182"/>
+      <c r="B113" s="185"/>
+      <c r="C113" s="182"/>
       <c r="D113" s="94"/>
-      <c r="E113" s="172"/>
+      <c r="E113" s="182"/>
       <c r="F113" s="63" t="s">
         <v>371</v>
       </c>
@@ -34735,17 +34741,17 @@
       <c r="Z113" s="7"/>
     </row>
     <row r="114" spans="1:26" ht="45" customHeight="1">
-      <c r="A114" s="171" t="s">
+      <c r="A114" s="181" t="s">
         <v>429</v>
       </c>
-      <c r="B114" s="173" t="s">
+      <c r="B114" s="184" t="s">
         <v>629</v>
       </c>
-      <c r="C114" s="171" t="s">
+      <c r="C114" s="181" t="s">
         <v>630</v>
       </c>
       <c r="D114" s="85"/>
-      <c r="E114" s="171" t="s">
+      <c r="E114" s="181" t="s">
         <v>614</v>
       </c>
       <c r="F114" s="46" t="s">
@@ -34763,7 +34769,7 @@
       </c>
       <c r="K114" s="85"/>
       <c r="L114" s="86"/>
-      <c r="M114" s="171" t="s">
+      <c r="M114" s="181" t="s">
         <v>614</v>
       </c>
       <c r="N114" s="102"/>
@@ -34781,11 +34787,11 @@
       <c r="Z114" s="7"/>
     </row>
     <row r="115" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A115" s="172"/>
-      <c r="B115" s="175"/>
-      <c r="C115" s="172"/>
+      <c r="A115" s="182"/>
+      <c r="B115" s="185"/>
+      <c r="C115" s="182"/>
       <c r="D115" s="94"/>
-      <c r="E115" s="172"/>
+      <c r="E115" s="182"/>
       <c r="F115" s="63" t="s">
         <v>392</v>
       </c>
@@ -34801,7 +34807,7 @@
       </c>
       <c r="K115" s="94"/>
       <c r="L115" s="89"/>
-      <c r="M115" s="172"/>
+      <c r="M115" s="182"/>
       <c r="N115" s="106"/>
       <c r="O115" s="7"/>
       <c r="P115" s="7"/>
@@ -34817,17 +34823,17 @@
       <c r="Z115" s="7"/>
     </row>
     <row r="116" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A116" s="171" t="s">
+      <c r="A116" s="181" t="s">
         <v>529</v>
       </c>
-      <c r="B116" s="173" t="s">
+      <c r="B116" s="184" t="s">
         <v>635</v>
       </c>
-      <c r="C116" s="171" t="s">
+      <c r="C116" s="181" t="s">
         <v>636</v>
       </c>
       <c r="D116" s="85"/>
-      <c r="E116" s="171" t="s">
+      <c r="E116" s="181" t="s">
         <v>614</v>
       </c>
       <c r="F116" s="46" t="s">
@@ -34845,7 +34851,7 @@
       </c>
       <c r="K116" s="85"/>
       <c r="L116" s="86"/>
-      <c r="M116" s="171" t="s">
+      <c r="M116" s="181" t="s">
         <v>614</v>
       </c>
       <c r="N116" s="102"/>
@@ -34863,11 +34869,11 @@
       <c r="Z116" s="7"/>
     </row>
     <row r="117" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A117" s="172"/>
-      <c r="B117" s="175"/>
-      <c r="C117" s="172"/>
+      <c r="A117" s="182"/>
+      <c r="B117" s="185"/>
+      <c r="C117" s="182"/>
       <c r="D117" s="94"/>
-      <c r="E117" s="172"/>
+      <c r="E117" s="182"/>
       <c r="F117" s="63" t="s">
         <v>412</v>
       </c>
@@ -34883,7 +34889,7 @@
       </c>
       <c r="K117" s="94"/>
       <c r="L117" s="89"/>
-      <c r="M117" s="172"/>
+      <c r="M117" s="182"/>
       <c r="N117" s="106"/>
       <c r="O117" s="7"/>
       <c r="P117" s="7"/>
@@ -34899,17 +34905,17 @@
       <c r="Z117" s="7"/>
     </row>
     <row r="118" spans="1:26" ht="30" customHeight="1">
-      <c r="A118" s="171" t="s">
+      <c r="A118" s="181" t="s">
         <v>641</v>
       </c>
-      <c r="B118" s="173" t="s">
+      <c r="B118" s="184" t="s">
         <v>642</v>
       </c>
-      <c r="C118" s="171" t="s">
+      <c r="C118" s="181" t="s">
         <v>643</v>
       </c>
       <c r="D118" s="85"/>
-      <c r="E118" s="171" t="s">
+      <c r="E118" s="181" t="s">
         <v>614</v>
       </c>
       <c r="F118" s="46" t="s">
@@ -34927,7 +34933,7 @@
       </c>
       <c r="K118" s="85"/>
       <c r="L118" s="86"/>
-      <c r="M118" s="171" t="s">
+      <c r="M118" s="181" t="s">
         <v>646</v>
       </c>
       <c r="N118" s="102"/>
@@ -34945,11 +34951,11 @@
       <c r="Z118" s="7"/>
     </row>
     <row r="119" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A119" s="170"/>
-      <c r="B119" s="174"/>
-      <c r="C119" s="170"/>
+      <c r="A119" s="180"/>
+      <c r="B119" s="186"/>
+      <c r="C119" s="180"/>
       <c r="D119" s="57"/>
-      <c r="E119" s="170"/>
+      <c r="E119" s="180"/>
       <c r="F119" s="53" t="s">
         <v>426</v>
       </c>
@@ -34965,7 +34971,7 @@
       </c>
       <c r="K119" s="57"/>
       <c r="L119" s="56"/>
-      <c r="M119" s="170"/>
+      <c r="M119" s="180"/>
       <c r="N119" s="103"/>
       <c r="O119" s="7"/>
       <c r="P119" s="7"/>
@@ -34981,11 +34987,11 @@
       <c r="Z119" s="7"/>
     </row>
     <row r="120" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A120" s="170"/>
-      <c r="B120" s="174"/>
-      <c r="C120" s="170"/>
+      <c r="A120" s="180"/>
+      <c r="B120" s="186"/>
+      <c r="C120" s="180"/>
       <c r="D120" s="57"/>
-      <c r="E120" s="170"/>
+      <c r="E120" s="180"/>
       <c r="F120" s="105" t="s">
         <v>433</v>
       </c>
@@ -35001,7 +35007,7 @@
       </c>
       <c r="K120" s="57"/>
       <c r="L120" s="56"/>
-      <c r="M120" s="170"/>
+      <c r="M120" s="180"/>
       <c r="N120" s="103"/>
       <c r="O120" s="7"/>
       <c r="P120" s="7"/>
@@ -35017,11 +35023,11 @@
       <c r="Z120" s="7"/>
     </row>
     <row r="121" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A121" s="170"/>
-      <c r="B121" s="174"/>
-      <c r="C121" s="170"/>
+      <c r="A121" s="180"/>
+      <c r="B121" s="186"/>
+      <c r="C121" s="180"/>
       <c r="D121" s="57"/>
-      <c r="E121" s="170"/>
+      <c r="E121" s="180"/>
       <c r="F121" s="53" t="s">
         <v>439</v>
       </c>
@@ -35037,7 +35043,7 @@
       </c>
       <c r="K121" s="57"/>
       <c r="L121" s="56"/>
-      <c r="M121" s="170"/>
+      <c r="M121" s="180"/>
       <c r="N121" s="103"/>
       <c r="O121" s="7"/>
       <c r="P121" s="7"/>
@@ -35053,11 +35059,11 @@
       <c r="Z121" s="7"/>
     </row>
     <row r="122" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A122" s="170"/>
-      <c r="B122" s="174"/>
-      <c r="C122" s="170"/>
+      <c r="A122" s="180"/>
+      <c r="B122" s="186"/>
+      <c r="C122" s="180"/>
       <c r="D122" s="57"/>
-      <c r="E122" s="170"/>
+      <c r="E122" s="180"/>
       <c r="F122" s="105" t="s">
         <v>451</v>
       </c>
@@ -35073,7 +35079,7 @@
       </c>
       <c r="K122" s="57"/>
       <c r="L122" s="56"/>
-      <c r="M122" s="170"/>
+      <c r="M122" s="180"/>
       <c r="N122" s="103"/>
       <c r="O122" s="7"/>
       <c r="P122" s="7"/>
@@ -35089,11 +35095,11 @@
       <c r="Z122" s="7"/>
     </row>
     <row r="123" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A123" s="172"/>
-      <c r="B123" s="175"/>
-      <c r="C123" s="172"/>
+      <c r="A123" s="182"/>
+      <c r="B123" s="185"/>
+      <c r="C123" s="182"/>
       <c r="D123" s="94"/>
-      <c r="E123" s="172"/>
+      <c r="E123" s="182"/>
       <c r="F123" s="63" t="s">
         <v>455</v>
       </c>
@@ -35109,7 +35115,7 @@
       </c>
       <c r="K123" s="94"/>
       <c r="L123" s="89"/>
-      <c r="M123" s="172"/>
+      <c r="M123" s="182"/>
       <c r="N123" s="106"/>
       <c r="O123" s="7"/>
       <c r="P123" s="7"/>
@@ -35125,17 +35131,17 @@
       <c r="Z123" s="7"/>
     </row>
     <row r="124" spans="1:26" ht="30" customHeight="1">
-      <c r="A124" s="171" t="s">
+      <c r="A124" s="181" t="s">
         <v>657</v>
       </c>
-      <c r="B124" s="173" t="s">
+      <c r="B124" s="184" t="s">
         <v>658</v>
       </c>
-      <c r="C124" s="171" t="s">
+      <c r="C124" s="181" t="s">
         <v>659</v>
       </c>
       <c r="D124" s="85"/>
-      <c r="E124" s="171" t="s">
+      <c r="E124" s="181" t="s">
         <v>614</v>
       </c>
       <c r="F124" s="46" t="s">
@@ -35153,7 +35159,7 @@
       </c>
       <c r="K124" s="85"/>
       <c r="L124" s="86"/>
-      <c r="M124" s="171" t="s">
+      <c r="M124" s="181" t="s">
         <v>614</v>
       </c>
       <c r="N124" s="102"/>
@@ -35171,11 +35177,11 @@
       <c r="Z124" s="7"/>
     </row>
     <row r="125" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A125" s="172"/>
-      <c r="B125" s="175"/>
-      <c r="C125" s="172"/>
+      <c r="A125" s="182"/>
+      <c r="B125" s="185"/>
+      <c r="C125" s="182"/>
       <c r="D125" s="94"/>
-      <c r="E125" s="172"/>
+      <c r="E125" s="182"/>
       <c r="F125" s="108" t="s">
         <v>465</v>
       </c>
@@ -35191,7 +35197,7 @@
       </c>
       <c r="K125" s="94"/>
       <c r="L125" s="89"/>
-      <c r="M125" s="172"/>
+      <c r="M125" s="182"/>
       <c r="N125" s="106"/>
       <c r="O125" s="7"/>
       <c r="P125" s="7"/>
@@ -35253,17 +35259,17 @@
       <c r="Z126" s="7"/>
     </row>
     <row r="127" spans="1:26" ht="36" customHeight="1">
-      <c r="A127" s="171" t="s">
+      <c r="A127" s="181" t="s">
         <v>669</v>
       </c>
-      <c r="B127" s="173" t="s">
+      <c r="B127" s="184" t="s">
         <v>670</v>
       </c>
-      <c r="C127" s="171" t="s">
+      <c r="C127" s="181" t="s">
         <v>671</v>
       </c>
       <c r="D127" s="85"/>
-      <c r="E127" s="171" t="s">
+      <c r="E127" s="181" t="s">
         <v>614</v>
       </c>
       <c r="F127" s="46" t="s">
@@ -35281,7 +35287,7 @@
       </c>
       <c r="K127" s="85"/>
       <c r="L127" s="86"/>
-      <c r="M127" s="171" t="s">
+      <c r="M127" s="181" t="s">
         <v>614</v>
       </c>
       <c r="N127" s="102"/>
@@ -35299,11 +35305,11 @@
       <c r="Z127" s="7"/>
     </row>
     <row r="128" spans="1:26" ht="26.25" customHeight="1">
-      <c r="A128" s="172"/>
-      <c r="B128" s="175"/>
-      <c r="C128" s="172"/>
+      <c r="A128" s="182"/>
+      <c r="B128" s="185"/>
+      <c r="C128" s="182"/>
       <c r="D128" s="94"/>
-      <c r="E128" s="172"/>
+      <c r="E128" s="182"/>
       <c r="F128" s="63" t="s">
         <v>478</v>
       </c>
@@ -35319,7 +35325,7 @@
       </c>
       <c r="K128" s="94"/>
       <c r="L128" s="89"/>
-      <c r="M128" s="172"/>
+      <c r="M128" s="182"/>
       <c r="N128" s="106"/>
       <c r="O128" s="7"/>
       <c r="P128" s="7"/>
@@ -35335,17 +35341,17 @@
       <c r="Z128" s="7"/>
     </row>
     <row r="129" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A129" s="171" t="s">
+      <c r="A129" s="181" t="s">
         <v>676</v>
       </c>
-      <c r="B129" s="173" t="s">
+      <c r="B129" s="184" t="s">
         <v>677</v>
       </c>
-      <c r="C129" s="171" t="s">
+      <c r="C129" s="181" t="s">
         <v>671</v>
       </c>
       <c r="D129" s="85"/>
-      <c r="E129" s="171" t="s">
+      <c r="E129" s="181" t="s">
         <v>614</v>
       </c>
       <c r="F129" s="46" t="s">
@@ -35363,7 +35369,7 @@
       </c>
       <c r="K129" s="85"/>
       <c r="L129" s="86"/>
-      <c r="M129" s="171" t="s">
+      <c r="M129" s="181" t="s">
         <v>614</v>
       </c>
       <c r="N129" s="102"/>
@@ -35381,11 +35387,11 @@
       <c r="Z129" s="7"/>
     </row>
     <row r="130" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A130" s="172"/>
-      <c r="B130" s="175"/>
-      <c r="C130" s="172"/>
+      <c r="A130" s="182"/>
+      <c r="B130" s="185"/>
+      <c r="C130" s="182"/>
       <c r="D130" s="94"/>
-      <c r="E130" s="172"/>
+      <c r="E130" s="182"/>
       <c r="F130" s="63" t="s">
         <v>488</v>
       </c>
@@ -35401,7 +35407,7 @@
       </c>
       <c r="K130" s="94"/>
       <c r="L130" s="89"/>
-      <c r="M130" s="172"/>
+      <c r="M130" s="182"/>
       <c r="N130" s="106"/>
       <c r="O130" s="7"/>
       <c r="P130" s="7"/>
@@ -35463,17 +35469,17 @@
       <c r="Z131" s="7"/>
     </row>
     <row r="132" spans="1:26" ht="60" customHeight="1">
-      <c r="A132" s="171" t="s">
+      <c r="A132" s="181" t="s">
         <v>687</v>
       </c>
-      <c r="B132" s="173" t="s">
+      <c r="B132" s="184" t="s">
         <v>688</v>
       </c>
-      <c r="C132" s="171" t="s">
+      <c r="C132" s="181" t="s">
         <v>689</v>
       </c>
       <c r="D132" s="85"/>
-      <c r="E132" s="171" t="s">
+      <c r="E132" s="181" t="s">
         <v>614</v>
       </c>
       <c r="F132" s="46" t="s">
@@ -35491,7 +35497,7 @@
       </c>
       <c r="K132" s="85"/>
       <c r="L132" s="86"/>
-      <c r="M132" s="171" t="s">
+      <c r="M132" s="181" t="s">
         <v>614</v>
       </c>
       <c r="N132" s="102"/>
@@ -35509,11 +35515,11 @@
       <c r="Z132" s="7"/>
     </row>
     <row r="133" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A133" s="170"/>
-      <c r="B133" s="174"/>
-      <c r="C133" s="170"/>
+      <c r="A133" s="180"/>
+      <c r="B133" s="186"/>
+      <c r="C133" s="180"/>
       <c r="D133" s="57"/>
-      <c r="E133" s="170"/>
+      <c r="E133" s="180"/>
       <c r="F133" s="53" t="s">
         <v>522</v>
       </c>
@@ -35529,7 +35535,7 @@
       </c>
       <c r="K133" s="57"/>
       <c r="L133" s="56"/>
-      <c r="M133" s="170"/>
+      <c r="M133" s="180"/>
       <c r="N133" s="103"/>
       <c r="O133" s="7"/>
       <c r="P133" s="7"/>
@@ -35545,11 +35551,11 @@
       <c r="Z133" s="7"/>
     </row>
     <row r="134" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A134" s="170"/>
-      <c r="B134" s="174"/>
-      <c r="C134" s="170"/>
+      <c r="A134" s="180"/>
+      <c r="B134" s="186"/>
+      <c r="C134" s="180"/>
       <c r="D134" s="57"/>
-      <c r="E134" s="170"/>
+      <c r="E134" s="180"/>
       <c r="F134" s="53" t="s">
         <v>532</v>
       </c>
@@ -35565,7 +35571,7 @@
       </c>
       <c r="K134" s="57"/>
       <c r="L134" s="56"/>
-      <c r="M134" s="170"/>
+      <c r="M134" s="180"/>
       <c r="N134" s="103"/>
       <c r="O134" s="7"/>
       <c r="P134" s="7"/>
@@ -35581,11 +35587,11 @@
       <c r="Z134" s="7"/>
     </row>
     <row r="135" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A135" s="172"/>
-      <c r="B135" s="175"/>
-      <c r="C135" s="172"/>
+      <c r="A135" s="182"/>
+      <c r="B135" s="185"/>
+      <c r="C135" s="182"/>
       <c r="D135" s="94"/>
-      <c r="E135" s="172"/>
+      <c r="E135" s="182"/>
       <c r="F135" s="63" t="s">
         <v>535</v>
       </c>
@@ -35601,7 +35607,7 @@
       </c>
       <c r="K135" s="94"/>
       <c r="L135" s="89"/>
-      <c r="M135" s="172"/>
+      <c r="M135" s="182"/>
       <c r="N135" s="106"/>
       <c r="O135" s="7"/>
       <c r="P135" s="7"/>
@@ -35617,17 +35623,17 @@
       <c r="Z135" s="7"/>
     </row>
     <row r="136" spans="1:26" ht="30" customHeight="1">
-      <c r="A136" s="171" t="s">
+      <c r="A136" s="181" t="s">
         <v>698</v>
       </c>
-      <c r="B136" s="173" t="s">
+      <c r="B136" s="184" t="s">
         <v>699</v>
       </c>
-      <c r="C136" s="171" t="s">
+      <c r="C136" s="181" t="s">
         <v>700</v>
       </c>
       <c r="D136" s="85"/>
-      <c r="E136" s="171" t="s">
+      <c r="E136" s="181" t="s">
         <v>614</v>
       </c>
       <c r="F136" s="46" t="s">
@@ -35645,7 +35651,7 @@
       </c>
       <c r="K136" s="85"/>
       <c r="L136" s="86"/>
-      <c r="M136" s="171" t="s">
+      <c r="M136" s="181" t="s">
         <v>614</v>
       </c>
       <c r="N136" s="102"/>
@@ -35663,11 +35669,11 @@
       <c r="Z136" s="7"/>
     </row>
     <row r="137" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A137" s="172"/>
-      <c r="B137" s="175"/>
-      <c r="C137" s="172"/>
+      <c r="A137" s="182"/>
+      <c r="B137" s="185"/>
+      <c r="C137" s="182"/>
       <c r="D137" s="94"/>
-      <c r="E137" s="172"/>
+      <c r="E137" s="182"/>
       <c r="F137" s="63" t="s">
         <v>543</v>
       </c>
@@ -35683,7 +35689,7 @@
       </c>
       <c r="K137" s="94"/>
       <c r="L137" s="89"/>
-      <c r="M137" s="172"/>
+      <c r="M137" s="182"/>
       <c r="N137" s="106"/>
       <c r="O137" s="7"/>
       <c r="P137" s="7"/>
@@ -35699,17 +35705,17 @@
       <c r="Z137" s="7"/>
     </row>
     <row r="138" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A138" s="171" t="s">
+      <c r="A138" s="181" t="s">
         <v>705</v>
       </c>
-      <c r="B138" s="173" t="s">
+      <c r="B138" s="184" t="s">
         <v>706</v>
       </c>
-      <c r="C138" s="171" t="s">
+      <c r="C138" s="181" t="s">
         <v>707</v>
       </c>
       <c r="D138" s="85"/>
-      <c r="E138" s="171" t="s">
+      <c r="E138" s="181" t="s">
         <v>614</v>
       </c>
       <c r="F138" s="46" t="s">
@@ -35727,7 +35733,7 @@
       </c>
       <c r="K138" s="85"/>
       <c r="L138" s="86"/>
-      <c r="M138" s="171" t="s">
+      <c r="M138" s="181" t="s">
         <v>614</v>
       </c>
       <c r="N138" s="102"/>
@@ -35745,11 +35751,11 @@
       <c r="Z138" s="7"/>
     </row>
     <row r="139" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A139" s="172"/>
-      <c r="B139" s="175"/>
-      <c r="C139" s="172"/>
+      <c r="A139" s="182"/>
+      <c r="B139" s="185"/>
+      <c r="C139" s="182"/>
       <c r="D139" s="94"/>
-      <c r="E139" s="172"/>
+      <c r="E139" s="182"/>
       <c r="F139" s="63" t="s">
         <v>711</v>
       </c>
@@ -35765,7 +35771,7 @@
       </c>
       <c r="K139" s="94"/>
       <c r="L139" s="89"/>
-      <c r="M139" s="172"/>
+      <c r="M139" s="182"/>
       <c r="N139" s="106"/>
       <c r="O139" s="7"/>
       <c r="P139" s="7"/>
@@ -35781,17 +35787,17 @@
       <c r="Z139" s="7"/>
     </row>
     <row r="140" spans="1:26" ht="30" customHeight="1">
-      <c r="A140" s="171" t="s">
+      <c r="A140" s="181" t="s">
         <v>714</v>
       </c>
-      <c r="B140" s="173" t="s">
+      <c r="B140" s="184" t="s">
         <v>715</v>
       </c>
-      <c r="C140" s="171" t="s">
+      <c r="C140" s="181" t="s">
         <v>716</v>
       </c>
       <c r="D140" s="85"/>
-      <c r="E140" s="171" t="s">
+      <c r="E140" s="181" t="s">
         <v>614</v>
       </c>
       <c r="F140" s="46" t="s">
@@ -35809,7 +35815,7 @@
       </c>
       <c r="K140" s="85"/>
       <c r="L140" s="86"/>
-      <c r="M140" s="171" t="s">
+      <c r="M140" s="181" t="s">
         <v>614</v>
       </c>
       <c r="N140" s="102"/>
@@ -35827,11 +35833,11 @@
       <c r="Z140" s="7"/>
     </row>
     <row r="141" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A141" s="172"/>
-      <c r="B141" s="175"/>
-      <c r="C141" s="172"/>
+      <c r="A141" s="182"/>
+      <c r="B141" s="185"/>
+      <c r="C141" s="182"/>
       <c r="D141" s="94"/>
-      <c r="E141" s="172"/>
+      <c r="E141" s="182"/>
       <c r="F141" s="63" t="s">
         <v>720</v>
       </c>
@@ -35847,7 +35853,7 @@
       </c>
       <c r="K141" s="94"/>
       <c r="L141" s="89"/>
-      <c r="M141" s="172"/>
+      <c r="M141" s="182"/>
       <c r="N141" s="106"/>
       <c r="O141" s="7"/>
       <c r="P141" s="7"/>
@@ -35863,17 +35869,17 @@
       <c r="Z141" s="7"/>
     </row>
     <row r="142" spans="1:26" ht="62.25" customHeight="1">
-      <c r="A142" s="171" t="s">
+      <c r="A142" s="181" t="s">
         <v>723</v>
       </c>
-      <c r="B142" s="173" t="s">
+      <c r="B142" s="184" t="s">
         <v>724</v>
       </c>
-      <c r="C142" s="171" t="s">
+      <c r="C142" s="181" t="s">
         <v>725</v>
       </c>
       <c r="D142" s="85"/>
-      <c r="E142" s="171" t="s">
+      <c r="E142" s="181" t="s">
         <v>726</v>
       </c>
       <c r="F142" s="46" t="s">
@@ -35891,7 +35897,7 @@
       </c>
       <c r="K142" s="85"/>
       <c r="L142" s="86"/>
-      <c r="M142" s="171" t="s">
+      <c r="M142" s="181" t="s">
         <v>726</v>
       </c>
       <c r="N142" s="102"/>
@@ -35909,11 +35915,11 @@
       <c r="Z142" s="7"/>
     </row>
     <row r="143" spans="1:26" ht="64.5" customHeight="1">
-      <c r="A143" s="172"/>
-      <c r="B143" s="175"/>
-      <c r="C143" s="172"/>
+      <c r="A143" s="182"/>
+      <c r="B143" s="185"/>
+      <c r="C143" s="182"/>
       <c r="D143" s="94"/>
-      <c r="E143" s="172"/>
+      <c r="E143" s="182"/>
       <c r="F143" s="63" t="s">
         <v>730</v>
       </c>
@@ -35929,7 +35935,7 @@
       </c>
       <c r="K143" s="94"/>
       <c r="L143" s="89"/>
-      <c r="M143" s="172"/>
+      <c r="M143" s="182"/>
       <c r="N143" s="106"/>
       <c r="O143" s="7"/>
       <c r="P143" s="7"/>
@@ -35945,17 +35951,17 @@
       <c r="Z143" s="7"/>
     </row>
     <row r="144" spans="1:26" ht="30" customHeight="1">
-      <c r="A144" s="171" t="s">
+      <c r="A144" s="181" t="s">
         <v>731</v>
       </c>
-      <c r="B144" s="173" t="s">
+      <c r="B144" s="184" t="s">
         <v>732</v>
       </c>
-      <c r="C144" s="171" t="s">
+      <c r="C144" s="181" t="s">
         <v>733</v>
       </c>
       <c r="D144" s="85"/>
-      <c r="E144" s="171" t="s">
+      <c r="E144" s="181" t="s">
         <v>726</v>
       </c>
       <c r="F144" s="46" t="s">
@@ -35973,7 +35979,7 @@
       </c>
       <c r="K144" s="85"/>
       <c r="L144" s="86"/>
-      <c r="M144" s="171" t="s">
+      <c r="M144" s="181" t="s">
         <v>726</v>
       </c>
       <c r="N144" s="102"/>
@@ -35991,11 +35997,11 @@
       <c r="Z144" s="7"/>
     </row>
     <row r="145" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A145" s="170"/>
-      <c r="B145" s="174"/>
-      <c r="C145" s="170"/>
+      <c r="A145" s="180"/>
+      <c r="B145" s="186"/>
+      <c r="C145" s="180"/>
       <c r="D145" s="57"/>
-      <c r="E145" s="170"/>
+      <c r="E145" s="180"/>
       <c r="F145" s="53" t="s">
         <v>737</v>
       </c>
@@ -36011,7 +36017,7 @@
       </c>
       <c r="K145" s="57"/>
       <c r="L145" s="56"/>
-      <c r="M145" s="170"/>
+      <c r="M145" s="180"/>
       <c r="N145" s="103"/>
       <c r="O145" s="7"/>
       <c r="P145" s="7"/>
@@ -36027,11 +36033,11 @@
       <c r="Z145" s="7"/>
     </row>
     <row r="146" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A146" s="170"/>
-      <c r="B146" s="174"/>
-      <c r="C146" s="170"/>
+      <c r="A146" s="180"/>
+      <c r="B146" s="186"/>
+      <c r="C146" s="180"/>
       <c r="D146" s="57"/>
-      <c r="E146" s="170"/>
+      <c r="E146" s="180"/>
       <c r="F146" s="53" t="s">
         <v>740</v>
       </c>
@@ -36047,7 +36053,7 @@
       </c>
       <c r="K146" s="57"/>
       <c r="L146" s="56"/>
-      <c r="M146" s="170"/>
+      <c r="M146" s="180"/>
       <c r="N146" s="103"/>
       <c r="O146" s="7"/>
       <c r="P146" s="7"/>
@@ -36063,11 +36069,11 @@
       <c r="Z146" s="7"/>
     </row>
     <row r="147" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A147" s="170"/>
-      <c r="B147" s="174"/>
-      <c r="C147" s="170"/>
+      <c r="A147" s="180"/>
+      <c r="B147" s="186"/>
+      <c r="C147" s="180"/>
       <c r="D147" s="57"/>
-      <c r="E147" s="170"/>
+      <c r="E147" s="180"/>
       <c r="F147" s="53" t="s">
         <v>743</v>
       </c>
@@ -36083,7 +36089,7 @@
       </c>
       <c r="K147" s="57"/>
       <c r="L147" s="56"/>
-      <c r="M147" s="170"/>
+      <c r="M147" s="180"/>
       <c r="N147" s="103"/>
       <c r="O147" s="7"/>
       <c r="P147" s="7"/>
@@ -36099,11 +36105,11 @@
       <c r="Z147" s="7"/>
     </row>
     <row r="148" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A148" s="170"/>
-      <c r="B148" s="174"/>
-      <c r="C148" s="170"/>
+      <c r="A148" s="180"/>
+      <c r="B148" s="186"/>
+      <c r="C148" s="180"/>
       <c r="D148" s="57"/>
-      <c r="E148" s="170"/>
+      <c r="E148" s="180"/>
       <c r="F148" s="53" t="s">
         <v>745</v>
       </c>
@@ -36119,7 +36125,7 @@
       </c>
       <c r="K148" s="57"/>
       <c r="L148" s="56"/>
-      <c r="M148" s="170"/>
+      <c r="M148" s="180"/>
       <c r="N148" s="103"/>
       <c r="O148" s="7"/>
       <c r="P148" s="7"/>
@@ -36135,11 +36141,11 @@
       <c r="Z148" s="7"/>
     </row>
     <row r="149" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A149" s="170"/>
-      <c r="B149" s="174"/>
-      <c r="C149" s="170"/>
+      <c r="A149" s="180"/>
+      <c r="B149" s="186"/>
+      <c r="C149" s="180"/>
       <c r="D149" s="57"/>
-      <c r="E149" s="170"/>
+      <c r="E149" s="180"/>
       <c r="F149" s="53" t="s">
         <v>748</v>
       </c>
@@ -36155,7 +36161,7 @@
       </c>
       <c r="K149" s="57"/>
       <c r="L149" s="56"/>
-      <c r="M149" s="170"/>
+      <c r="M149" s="180"/>
       <c r="N149" s="103"/>
       <c r="O149" s="7"/>
       <c r="P149" s="7"/>
@@ -36171,11 +36177,11 @@
       <c r="Z149" s="7"/>
     </row>
     <row r="150" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A150" s="170"/>
-      <c r="B150" s="174"/>
-      <c r="C150" s="170"/>
+      <c r="A150" s="180"/>
+      <c r="B150" s="186"/>
+      <c r="C150" s="180"/>
       <c r="D150" s="57"/>
-      <c r="E150" s="170"/>
+      <c r="E150" s="180"/>
       <c r="F150" s="53" t="s">
         <v>751</v>
       </c>
@@ -36191,7 +36197,7 @@
       </c>
       <c r="K150" s="57"/>
       <c r="L150" s="56"/>
-      <c r="M150" s="170"/>
+      <c r="M150" s="180"/>
       <c r="N150" s="103"/>
       <c r="O150" s="7"/>
       <c r="P150" s="7"/>
@@ -36207,11 +36213,11 @@
       <c r="Z150" s="7"/>
     </row>
     <row r="151" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A151" s="172"/>
-      <c r="B151" s="175"/>
-      <c r="C151" s="172"/>
+      <c r="A151" s="182"/>
+      <c r="B151" s="185"/>
+      <c r="C151" s="182"/>
       <c r="D151" s="94"/>
-      <c r="E151" s="172"/>
+      <c r="E151" s="182"/>
       <c r="F151" s="63" t="s">
         <v>754</v>
       </c>
@@ -36227,7 +36233,7 @@
       </c>
       <c r="K151" s="94"/>
       <c r="L151" s="89"/>
-      <c r="M151" s="172"/>
+      <c r="M151" s="182"/>
       <c r="N151" s="106"/>
       <c r="O151" s="7"/>
       <c r="P151" s="7"/>
@@ -36243,17 +36249,17 @@
       <c r="Z151" s="7"/>
     </row>
     <row r="152" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A152" s="171" t="s">
+      <c r="A152" s="181" t="s">
         <v>757</v>
       </c>
-      <c r="B152" s="173" t="s">
+      <c r="B152" s="184" t="s">
         <v>758</v>
       </c>
-      <c r="C152" s="171" t="s">
+      <c r="C152" s="181" t="s">
         <v>759</v>
       </c>
       <c r="D152" s="85"/>
-      <c r="E152" s="171" t="s">
+      <c r="E152" s="181" t="s">
         <v>726</v>
       </c>
       <c r="F152" s="46" t="s">
@@ -36271,7 +36277,7 @@
       </c>
       <c r="K152" s="85"/>
       <c r="L152" s="86"/>
-      <c r="M152" s="171" t="s">
+      <c r="M152" s="181" t="s">
         <v>726</v>
       </c>
       <c r="N152" s="102"/>
@@ -36289,11 +36295,11 @@
       <c r="Z152" s="7"/>
     </row>
     <row r="153" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A153" s="170"/>
-      <c r="B153" s="174"/>
-      <c r="C153" s="170"/>
+      <c r="A153" s="180"/>
+      <c r="B153" s="186"/>
+      <c r="C153" s="180"/>
       <c r="D153" s="57"/>
-      <c r="E153" s="170"/>
+      <c r="E153" s="180"/>
       <c r="F153" s="53" t="s">
         <v>763</v>
       </c>
@@ -36309,7 +36315,7 @@
       </c>
       <c r="K153" s="57"/>
       <c r="L153" s="56"/>
-      <c r="M153" s="170"/>
+      <c r="M153" s="180"/>
       <c r="N153" s="103"/>
       <c r="O153" s="7"/>
       <c r="P153" s="7"/>
@@ -36325,11 +36331,11 @@
       <c r="Z153" s="7"/>
     </row>
     <row r="154" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A154" s="172"/>
-      <c r="B154" s="175"/>
-      <c r="C154" s="172"/>
+      <c r="A154" s="182"/>
+      <c r="B154" s="185"/>
+      <c r="C154" s="182"/>
       <c r="D154" s="94"/>
-      <c r="E154" s="172"/>
+      <c r="E154" s="182"/>
       <c r="F154" s="63" t="s">
         <v>766</v>
       </c>
@@ -36345,7 +36351,7 @@
       </c>
       <c r="K154" s="94"/>
       <c r="L154" s="89"/>
-      <c r="M154" s="172"/>
+      <c r="M154" s="182"/>
       <c r="N154" s="106"/>
       <c r="O154" s="7"/>
       <c r="P154" s="7"/>
@@ -42608,6 +42614,107 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="125">
+    <mergeCell ref="C22:C32"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="C116:C117"/>
+    <mergeCell ref="C118:C123"/>
+    <mergeCell ref="B106:B113"/>
+    <mergeCell ref="B132:B135"/>
+    <mergeCell ref="B129:B130"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="B37:B47"/>
+    <mergeCell ref="B118:B123"/>
+    <mergeCell ref="B124:B125"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B22:B32"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="B76:B87"/>
+    <mergeCell ref="B116:B117"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B127:B128"/>
+    <mergeCell ref="C106:C113"/>
+    <mergeCell ref="C114:C115"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="B48:B61"/>
+    <mergeCell ref="B62:B75"/>
+    <mergeCell ref="B88:B105"/>
+    <mergeCell ref="B114:B115"/>
+    <mergeCell ref="M7:M10"/>
+    <mergeCell ref="M12:M16"/>
+    <mergeCell ref="E12:E16"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E37:E47"/>
+    <mergeCell ref="E33:E36"/>
+    <mergeCell ref="E23:E32"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="E48:E61"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="M106:M112"/>
+    <mergeCell ref="M63:M75"/>
+    <mergeCell ref="C33:C36"/>
+    <mergeCell ref="C48:C61"/>
+    <mergeCell ref="C37:C47"/>
+    <mergeCell ref="C76:C87"/>
+    <mergeCell ref="C62:C75"/>
+    <mergeCell ref="M76:M86"/>
+    <mergeCell ref="M33:M36"/>
+    <mergeCell ref="M49:M61"/>
+    <mergeCell ref="M37:M46"/>
+    <mergeCell ref="M18:M21"/>
+    <mergeCell ref="M22:M31"/>
+    <mergeCell ref="M144:M151"/>
+    <mergeCell ref="M142:M143"/>
+    <mergeCell ref="M132:M135"/>
+    <mergeCell ref="M136:M137"/>
+    <mergeCell ref="M118:M123"/>
+    <mergeCell ref="M116:M117"/>
+    <mergeCell ref="M124:M125"/>
+    <mergeCell ref="M152:M154"/>
+    <mergeCell ref="M127:M128"/>
+    <mergeCell ref="A88:A105"/>
+    <mergeCell ref="A76:A87"/>
+    <mergeCell ref="A118:A123"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A129:A130"/>
+    <mergeCell ref="A127:A128"/>
+    <mergeCell ref="A138:A139"/>
+    <mergeCell ref="A142:A143"/>
+    <mergeCell ref="A152:A154"/>
+    <mergeCell ref="A144:A151"/>
+    <mergeCell ref="A140:A141"/>
+    <mergeCell ref="M114:M115"/>
+    <mergeCell ref="M88:M103"/>
+    <mergeCell ref="M129:M130"/>
+    <mergeCell ref="M138:M139"/>
+    <mergeCell ref="M140:M141"/>
+    <mergeCell ref="E124:E125"/>
+    <mergeCell ref="E132:E135"/>
+    <mergeCell ref="B144:B151"/>
+    <mergeCell ref="B138:B139"/>
+    <mergeCell ref="B142:B143"/>
+    <mergeCell ref="B152:B154"/>
+    <mergeCell ref="B140:B141"/>
+    <mergeCell ref="E142:E143"/>
+    <mergeCell ref="E144:E151"/>
+    <mergeCell ref="E116:E117"/>
+    <mergeCell ref="E127:E128"/>
+    <mergeCell ref="C152:C154"/>
+    <mergeCell ref="E152:E154"/>
+    <mergeCell ref="E140:E141"/>
+    <mergeCell ref="C142:C143"/>
+    <mergeCell ref="C144:C151"/>
+    <mergeCell ref="C140:C141"/>
+    <mergeCell ref="C138:C139"/>
+    <mergeCell ref="E138:E139"/>
+    <mergeCell ref="E129:E130"/>
+    <mergeCell ref="B136:B137"/>
+    <mergeCell ref="C129:C130"/>
+    <mergeCell ref="C132:C135"/>
+    <mergeCell ref="C136:C137"/>
+    <mergeCell ref="C127:C128"/>
+    <mergeCell ref="C124:C125"/>
     <mergeCell ref="E76:E87"/>
     <mergeCell ref="E62:E75"/>
     <mergeCell ref="E88:E105"/>
@@ -42632,107 +42739,6 @@
     <mergeCell ref="A106:A113"/>
     <mergeCell ref="C88:C105"/>
     <mergeCell ref="C1:C4"/>
-    <mergeCell ref="B140:B141"/>
-    <mergeCell ref="E142:E143"/>
-    <mergeCell ref="E144:E151"/>
-    <mergeCell ref="E116:E117"/>
-    <mergeCell ref="E127:E128"/>
-    <mergeCell ref="C152:C154"/>
-    <mergeCell ref="E152:E154"/>
-    <mergeCell ref="E140:E141"/>
-    <mergeCell ref="C142:C143"/>
-    <mergeCell ref="C144:C151"/>
-    <mergeCell ref="C140:C141"/>
-    <mergeCell ref="C138:C139"/>
-    <mergeCell ref="E138:E139"/>
-    <mergeCell ref="E129:E130"/>
-    <mergeCell ref="B136:B137"/>
-    <mergeCell ref="C129:C130"/>
-    <mergeCell ref="C132:C135"/>
-    <mergeCell ref="C136:C137"/>
-    <mergeCell ref="C127:C128"/>
-    <mergeCell ref="C124:C125"/>
-    <mergeCell ref="M152:M154"/>
-    <mergeCell ref="M127:M128"/>
-    <mergeCell ref="A88:A105"/>
-    <mergeCell ref="A76:A87"/>
-    <mergeCell ref="A118:A123"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A129:A130"/>
-    <mergeCell ref="A127:A128"/>
-    <mergeCell ref="A138:A139"/>
-    <mergeCell ref="A142:A143"/>
-    <mergeCell ref="A152:A154"/>
-    <mergeCell ref="A144:A151"/>
-    <mergeCell ref="A140:A141"/>
-    <mergeCell ref="M114:M115"/>
-    <mergeCell ref="M88:M103"/>
-    <mergeCell ref="M129:M130"/>
-    <mergeCell ref="M138:M139"/>
-    <mergeCell ref="M140:M141"/>
-    <mergeCell ref="E124:E125"/>
-    <mergeCell ref="E132:E135"/>
-    <mergeCell ref="B144:B151"/>
-    <mergeCell ref="B138:B139"/>
-    <mergeCell ref="B142:B143"/>
-    <mergeCell ref="B152:B154"/>
-    <mergeCell ref="M18:M21"/>
-    <mergeCell ref="M22:M31"/>
-    <mergeCell ref="M144:M151"/>
-    <mergeCell ref="M142:M143"/>
-    <mergeCell ref="M132:M135"/>
-    <mergeCell ref="M136:M137"/>
-    <mergeCell ref="M118:M123"/>
-    <mergeCell ref="M116:M117"/>
-    <mergeCell ref="M124:M125"/>
-    <mergeCell ref="B62:B75"/>
-    <mergeCell ref="B88:B105"/>
-    <mergeCell ref="B114:B115"/>
-    <mergeCell ref="M7:M10"/>
-    <mergeCell ref="M12:M16"/>
-    <mergeCell ref="E12:E16"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="E37:E47"/>
-    <mergeCell ref="E33:E36"/>
-    <mergeCell ref="E23:E32"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="E48:E61"/>
-    <mergeCell ref="C12:C16"/>
-    <mergeCell ref="M106:M112"/>
-    <mergeCell ref="M63:M75"/>
-    <mergeCell ref="C33:C36"/>
-    <mergeCell ref="C48:C61"/>
-    <mergeCell ref="C37:C47"/>
-    <mergeCell ref="C76:C87"/>
-    <mergeCell ref="C62:C75"/>
-    <mergeCell ref="M76:M86"/>
-    <mergeCell ref="M33:M36"/>
-    <mergeCell ref="M49:M61"/>
-    <mergeCell ref="M37:M46"/>
-    <mergeCell ref="C22:C32"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="C116:C117"/>
-    <mergeCell ref="C118:C123"/>
-    <mergeCell ref="B106:B113"/>
-    <mergeCell ref="B132:B135"/>
-    <mergeCell ref="B129:B130"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="B37:B47"/>
-    <mergeCell ref="B118:B123"/>
-    <mergeCell ref="B124:B125"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="B22:B32"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="B76:B87"/>
-    <mergeCell ref="B116:B117"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B127:B128"/>
-    <mergeCell ref="C106:C113"/>
-    <mergeCell ref="C114:C115"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="B48:B61"/>
   </mergeCells>
   <conditionalFormatting sqref="J7:J154">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">

</xml_diff>